<commit_message>
implemantando botoes de combinaçao
</commit_message>
<xml_diff>
--- a/dashboards_II.xlsx
+++ b/dashboards_II.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c548d412d6f19400/Área de Trabalho/Alura/excel/Projetos Git/04. DashBoard Especialista/02.Dashboard 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{8621F33A-E581-4B2B-8C24-DD17DCFBD997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3421F1DA-5902-47DB-8CF4-EA0047637F4F}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{8621F33A-E581-4B2B-8C24-DD17DCFBD997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30F779A2-12AD-458E-BC43-A4BCA92671B7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="3" xr2:uid="{18B12833-7551-4467-B611-A6E8F662E40B}"/>
   </bookViews>
@@ -788,15 +788,15 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="16" fmlaRange="ListaEstados" sel="0" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="16" fmlaLink="Auxiliar!$I$6" fmlaRange="ListaEstados" sel="5" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="5" dropStyle="combo" dx="16" fmlaRange="ListaAnos" sel="0" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="5" dropStyle="combo" dx="16" fmlaLink="Auxiliar!$K$6" fmlaRange="ListaAnos" sel="2" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="12" dropStyle="combo" dx="16" fmlaRange="ListaMeses" sel="0" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="12" dropStyle="combo" dx="16" fmlaLink="Auxiliar!$L$5" fmlaRange="ListaMeses" sel="3" val="0"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -22056,7 +22056,9 @@
       <c r="I5" s="35"/>
       <c r="J5" s="36"/>
       <c r="K5" s="23"/>
-      <c r="L5" s="30"/>
+      <c r="L5" s="30">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" s="17" t="s">
@@ -22070,9 +22072,13 @@
       <c r="H6" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="I6" s="37"/>
+      <c r="I6" s="37">
+        <v>5</v>
+      </c>
       <c r="J6" s="37"/>
-      <c r="K6" s="30"/>
+      <c r="K6" s="30">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="17" t="s">
@@ -22669,7 +22675,7 @@
   <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="Q8" sqref="Q7:Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Implemantendo os primeiros calculos
</commit_message>
<xml_diff>
--- a/dashboards_II.xlsx
+++ b/dashboards_II.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c548d412d6f19400/Área de Trabalho/Alura/excel/Projetos Git/04. DashBoard Especialista/02.Dashboard 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{8621F33A-E581-4B2B-8C24-DD17DCFBD997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30F779A2-12AD-458E-BC43-A4BCA92671B7}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{8621F33A-E581-4B2B-8C24-DD17DCFBD997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32080113-628C-44C4-9BB5-2CC7BFDC9576}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="3" xr2:uid="{18B12833-7551-4467-B611-A6E8F662E40B}"/>
   </bookViews>
@@ -82,6 +82,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -792,11 +814,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="5" dropStyle="combo" dx="16" fmlaLink="Auxiliar!$K$6" fmlaRange="ListaAnos" sel="2" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="5" dropStyle="combo" dx="16" fmlaLink="Auxiliar!$K$6" fmlaRange="ListaAnos" sel="1" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="12" dropStyle="combo" dx="16" fmlaLink="Auxiliar!$L$5" fmlaRange="ListaMeses" sel="3" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="12" dropStyle="combo" dx="16" fmlaLink="Auxiliar!$L$5" fmlaRange="ListaMeses" sel="6" val="0"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2338,7 +2360,7 @@
   <dimension ref="A1:L477"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -21945,8 +21967,8 @@
   </sheetPr>
   <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22045,7 +22067,10 @@
       <c r="A5" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="16"/>
+      <c r="B5" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A5,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
+        <v>0</v>
+      </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
       <c r="E5" s="24"/>
@@ -22053,18 +22078,27 @@
       <c r="H5" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="I5" s="35"/>
+      <c r="I5" s="35" t="str" cm="1">
+        <f t="array" ref="I5">INDEX(Auxiliar!ListaEstados,Auxiliar!IndiceEstado)</f>
+        <v>Bahia</v>
+      </c>
       <c r="J5" s="36"/>
-      <c r="K5" s="23"/>
+      <c r="K5" s="23" cm="1">
+        <f t="array" ref="K5">INDEX(Auxiliar!ListaAnos,Auxiliar!IndiceAno)</f>
+        <v>2018</v>
+      </c>
       <c r="L5" s="30">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="16"/>
+      <c r="B6" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A6,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
+        <v>0</v>
+      </c>
       <c r="C6" s="20"/>
       <c r="D6" s="20"/>
       <c r="E6" s="24"/>
@@ -22077,14 +22111,17 @@
       </c>
       <c r="J6" s="37"/>
       <c r="K6" s="30">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="16"/>
+      <c r="B7" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A7,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
+        <v>0</v>
+      </c>
       <c r="C7" s="20"/>
       <c r="D7" s="20"/>
       <c r="E7" s="24"/>
@@ -22094,7 +22131,10 @@
       <c r="A8" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="16"/>
+      <c r="B8" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A8,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
+        <v>0</v>
+      </c>
       <c r="C8" s="20"/>
       <c r="D8" s="20"/>
       <c r="E8" s="24"/>
@@ -22104,7 +22144,10 @@
       <c r="A9" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="16"/>
+      <c r="B9" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A9,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
+        <v>0</v>
+      </c>
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
       <c r="E9" s="24"/>
@@ -22128,7 +22171,10 @@
       <c r="A10" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="16"/>
+      <c r="B10" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A10,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
+        <v>0</v>
+      </c>
       <c r="C10" s="20"/>
       <c r="D10" s="20"/>
       <c r="E10" s="24"/>
@@ -22150,7 +22196,10 @@
       <c r="A11" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="16"/>
+      <c r="B11" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A11,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
+        <v>0</v>
+      </c>
       <c r="C11" s="20"/>
       <c r="D11" s="20"/>
       <c r="E11" s="24"/>
@@ -22172,7 +22221,10 @@
       <c r="A12" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="16"/>
+      <c r="B12" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A12,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
+        <v>9880</v>
+      </c>
       <c r="C12" s="20"/>
       <c r="D12" s="20"/>
       <c r="E12" s="24"/>
@@ -22194,7 +22246,10 @@
       <c r="A13" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="16"/>
+      <c r="B13" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A13,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
+        <v>3200</v>
+      </c>
       <c r="C13" s="20"/>
       <c r="D13" s="20"/>
       <c r="E13" s="24"/>
@@ -22214,7 +22269,10 @@
       <c r="A14" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="16"/>
+      <c r="B14" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A14,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
+        <v>0</v>
+      </c>
       <c r="C14" s="20"/>
       <c r="D14" s="20"/>
       <c r="E14" s="24"/>
@@ -22234,7 +22292,10 @@
       <c r="A15" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="16"/>
+      <c r="B15" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A15,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
+        <v>0</v>
+      </c>
       <c r="C15" s="20"/>
       <c r="D15" s="20"/>
       <c r="E15" s="24"/>
@@ -22254,7 +22315,10 @@
       <c r="A16" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="16"/>
+      <c r="B16" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A16,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
+        <v>0</v>
+      </c>
       <c r="C16" s="20"/>
       <c r="D16" s="20"/>
       <c r="E16" s="24"/>
@@ -22274,7 +22338,10 @@
       <c r="A17" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="16"/>
+      <c r="B17" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A17,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
+        <v>16455</v>
+      </c>
       <c r="C17" s="20"/>
       <c r="D17" s="20"/>
       <c r="E17" s="24"/>
@@ -22294,7 +22361,10 @@
       <c r="A18" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="16"/>
+      <c r="B18" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A18,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
+        <v>0</v>
+      </c>
       <c r="C18" s="20"/>
       <c r="D18" s="20"/>
       <c r="E18" s="24"/>
@@ -22314,7 +22384,10 @@
       <c r="A19" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="16"/>
+      <c r="B19" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A19,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
+        <v>0</v>
+      </c>
       <c r="C19" s="20"/>
       <c r="D19" s="20"/>
       <c r="E19" s="24"/>
@@ -22334,7 +22407,10 @@
       <c r="A20" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="16"/>
+      <c r="B20" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A20,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
+        <v>0</v>
+      </c>
       <c r="C20" s="20"/>
       <c r="D20" s="20"/>
       <c r="E20" s="24"/>
@@ -22348,7 +22424,10 @@
       <c r="A21" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="16"/>
+      <c r="B21" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A21,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
+        <v>0</v>
+      </c>
       <c r="C21" s="20"/>
       <c r="D21" s="20"/>
       <c r="E21" s="24"/>
@@ -22359,7 +22438,7 @@
       </c>
       <c r="K21" s="33" t="str">
         <f>"Análise de Vendas "&amp;Estado</f>
-        <v xml:space="preserve">Análise de Vendas </v>
+        <v>Análise de Vendas Bahia</v>
       </c>
       <c r="L21" s="33"/>
       <c r="M21" s="33"/>
@@ -22369,7 +22448,10 @@
       <c r="A22" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="16"/>
+      <c r="B22" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A22,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
+        <v>0</v>
+      </c>
       <c r="C22" s="20"/>
       <c r="D22" s="20"/>
       <c r="E22" s="24"/>
@@ -22395,7 +22477,10 @@
       <c r="A23" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="16"/>
+      <c r="B23" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A23,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
+        <v>33470</v>
+      </c>
       <c r="C23" s="20"/>
       <c r="D23" s="20"/>
       <c r="E23" s="24"/>
@@ -22413,7 +22498,10 @@
       <c r="A24" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="16"/>
+      <c r="B24" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A24,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
+        <v>0</v>
+      </c>
       <c r="C24" s="20"/>
       <c r="D24" s="20"/>
       <c r="E24" s="24"/>
@@ -22435,7 +22523,10 @@
       <c r="A25" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="16"/>
+      <c r="B25" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A25,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
+        <v>0</v>
+      </c>
       <c r="C25" s="20"/>
       <c r="D25" s="20"/>
       <c r="E25" s="24"/>
@@ -22457,7 +22548,10 @@
       <c r="A26" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="16"/>
+      <c r="B26" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A26,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
+        <v>0</v>
+      </c>
       <c r="C26" s="20"/>
       <c r="D26" s="20"/>
       <c r="E26" s="24"/>
@@ -22479,7 +22573,10 @@
       <c r="A27" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="16"/>
+      <c r="B27" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A27,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
+        <v>0</v>
+      </c>
       <c r="C27" s="20"/>
       <c r="D27" s="20"/>
       <c r="E27" s="24"/>
@@ -22501,7 +22598,10 @@
       <c r="A28" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="16"/>
+      <c r="B28" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A28,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
+        <v>0</v>
+      </c>
       <c r="C28" s="20"/>
       <c r="D28" s="20"/>
       <c r="E28" s="24"/>
@@ -22523,7 +22623,10 @@
       <c r="A29" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="16"/>
+      <c r="B29" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A29,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
+        <v>36670</v>
+      </c>
       <c r="C29" s="20"/>
       <c r="D29" s="20"/>
       <c r="E29" s="24"/>
@@ -22541,7 +22644,10 @@
       <c r="A30" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B30" s="16"/>
+      <c r="B30" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A30,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
+        <v>0</v>
+      </c>
       <c r="C30" s="20"/>
       <c r="D30" s="20"/>
       <c r="E30" s="24"/>
@@ -22563,7 +22669,10 @@
       <c r="A31" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="16"/>
+      <c r="B31" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A31,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
+        <v>0</v>
+      </c>
       <c r="C31" s="20"/>
       <c r="D31" s="20"/>
       <c r="E31" s="24"/>

</xml_diff>

<commit_message>
Implementando contses para analises de canceladas
</commit_message>
<xml_diff>
--- a/dashboards_II.xlsx
+++ b/dashboards_II.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c548d412d6f19400/Área de Trabalho/Alura/excel/Projetos Git/04. DashBoard Especialista/02.Dashboard 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{8621F33A-E581-4B2B-8C24-DD17DCFBD997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32080113-628C-44C4-9BB5-2CC7BFDC9576}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{8621F33A-E581-4B2B-8C24-DD17DCFBD997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA7B101C-C721-467E-9FA7-C9F568E15A76}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="3" xr2:uid="{18B12833-7551-4467-B611-A6E8F662E40B}"/>
   </bookViews>
@@ -21968,7 +21968,7 @@
   <dimension ref="A1:S39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6:J6"/>
+      <selection activeCell="C5" sqref="C5:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22071,7 +22071,10 @@
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A5,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
         <v>0</v>
       </c>
-      <c r="C5" s="20"/>
+      <c r="C5" s="20">
+        <f>COUNTIFS(Reservas[Estado],A5,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
+        <v>0</v>
+      </c>
       <c r="D5" s="20"/>
       <c r="E5" s="24"/>
       <c r="F5" s="25"/>
@@ -22099,7 +22102,10 @@
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A6,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
         <v>0</v>
       </c>
-      <c r="C6" s="20"/>
+      <c r="C6" s="20">
+        <f>COUNTIFS(Reservas[Estado],A6,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
+        <v>0</v>
+      </c>
       <c r="D6" s="20"/>
       <c r="E6" s="24"/>
       <c r="F6" s="25"/>
@@ -22122,7 +22128,10 @@
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A7,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
         <v>0</v>
       </c>
-      <c r="C7" s="20"/>
+      <c r="C7" s="20">
+        <f>COUNTIFS(Reservas[Estado],A7,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
+        <v>0</v>
+      </c>
       <c r="D7" s="20"/>
       <c r="E7" s="24"/>
       <c r="F7" s="25"/>
@@ -22135,7 +22144,10 @@
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A8,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
         <v>0</v>
       </c>
-      <c r="C8" s="20"/>
+      <c r="C8" s="20">
+        <f>COUNTIFS(Reservas[Estado],A8,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
+        <v>0</v>
+      </c>
       <c r="D8" s="20"/>
       <c r="E8" s="24"/>
       <c r="F8" s="25"/>
@@ -22148,7 +22160,10 @@
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A9,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
         <v>0</v>
       </c>
-      <c r="C9" s="20"/>
+      <c r="C9" s="20">
+        <f>COUNTIFS(Reservas[Estado],A9,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
+        <v>0</v>
+      </c>
       <c r="D9" s="20"/>
       <c r="E9" s="24"/>
       <c r="F9" s="25"/>
@@ -22175,7 +22190,10 @@
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A10,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
         <v>0</v>
       </c>
-      <c r="C10" s="20"/>
+      <c r="C10" s="20">
+        <f>COUNTIFS(Reservas[Estado],A10,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
+        <v>0</v>
+      </c>
       <c r="D10" s="20"/>
       <c r="E10" s="24"/>
       <c r="F10" s="25"/>
@@ -22200,7 +22218,10 @@
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A11,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
         <v>0</v>
       </c>
-      <c r="C11" s="20"/>
+      <c r="C11" s="20">
+        <f>COUNTIFS(Reservas[Estado],A11,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
+        <v>0</v>
+      </c>
       <c r="D11" s="20"/>
       <c r="E11" s="24"/>
       <c r="F11" s="25"/>
@@ -22225,7 +22246,10 @@
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A12,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
         <v>9880</v>
       </c>
-      <c r="C12" s="20"/>
+      <c r="C12" s="20">
+        <f>COUNTIFS(Reservas[Estado],A12,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
+        <v>2</v>
+      </c>
       <c r="D12" s="20"/>
       <c r="E12" s="24"/>
       <c r="F12" s="25"/>
@@ -22250,7 +22274,10 @@
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A13,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
         <v>3200</v>
       </c>
-      <c r="C13" s="20"/>
+      <c r="C13" s="20">
+        <f>COUNTIFS(Reservas[Estado],A13,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
+        <v>0</v>
+      </c>
       <c r="D13" s="20"/>
       <c r="E13" s="24"/>
       <c r="F13" s="25"/>
@@ -22273,7 +22300,10 @@
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A14,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
         <v>0</v>
       </c>
-      <c r="C14" s="20"/>
+      <c r="C14" s="20">
+        <f>COUNTIFS(Reservas[Estado],A14,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
+        <v>0</v>
+      </c>
       <c r="D14" s="20"/>
       <c r="E14" s="24"/>
       <c r="F14" s="25"/>
@@ -22296,7 +22326,10 @@
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A15,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
         <v>0</v>
       </c>
-      <c r="C15" s="20"/>
+      <c r="C15" s="20">
+        <f>COUNTIFS(Reservas[Estado],A15,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
+        <v>0</v>
+      </c>
       <c r="D15" s="20"/>
       <c r="E15" s="24"/>
       <c r="F15" s="25"/>
@@ -22319,7 +22352,10 @@
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A16,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
         <v>0</v>
       </c>
-      <c r="C16" s="20"/>
+      <c r="C16" s="20">
+        <f>COUNTIFS(Reservas[Estado],A16,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
+        <v>0</v>
+      </c>
       <c r="D16" s="20"/>
       <c r="E16" s="24"/>
       <c r="F16" s="25"/>
@@ -22342,7 +22378,10 @@
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A17,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
         <v>16455</v>
       </c>
-      <c r="C17" s="20"/>
+      <c r="C17" s="20">
+        <f>COUNTIFS(Reservas[Estado],A17,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
+        <v>2</v>
+      </c>
       <c r="D17" s="20"/>
       <c r="E17" s="24"/>
       <c r="F17" s="25"/>
@@ -22365,7 +22404,10 @@
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A18,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
         <v>0</v>
       </c>
-      <c r="C18" s="20"/>
+      <c r="C18" s="20">
+        <f>COUNTIFS(Reservas[Estado],A18,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
+        <v>0</v>
+      </c>
       <c r="D18" s="20"/>
       <c r="E18" s="24"/>
       <c r="F18" s="25"/>
@@ -22388,7 +22430,10 @@
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A19,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
         <v>0</v>
       </c>
-      <c r="C19" s="20"/>
+      <c r="C19" s="20">
+        <f>COUNTIFS(Reservas[Estado],A19,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
+        <v>0</v>
+      </c>
       <c r="D19" s="20"/>
       <c r="E19" s="24"/>
       <c r="F19" s="25"/>
@@ -22411,7 +22456,10 @@
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A20,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
         <v>0</v>
       </c>
-      <c r="C20" s="20"/>
+      <c r="C20" s="20">
+        <f>COUNTIFS(Reservas[Estado],A20,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
+        <v>0</v>
+      </c>
       <c r="D20" s="20"/>
       <c r="E20" s="24"/>
       <c r="F20" s="25"/>
@@ -22428,7 +22476,10 @@
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A21,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
         <v>0</v>
       </c>
-      <c r="C21" s="20"/>
+      <c r="C21" s="20">
+        <f>COUNTIFS(Reservas[Estado],A21,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
+        <v>0</v>
+      </c>
       <c r="D21" s="20"/>
       <c r="E21" s="24"/>
       <c r="F21" s="25"/>
@@ -22452,7 +22503,10 @@
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A22,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
         <v>0</v>
       </c>
-      <c r="C22" s="20"/>
+      <c r="C22" s="20">
+        <f>COUNTIFS(Reservas[Estado],A22,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
+        <v>0</v>
+      </c>
       <c r="D22" s="20"/>
       <c r="E22" s="24"/>
       <c r="F22" s="25"/>
@@ -22481,7 +22535,10 @@
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A23,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
         <v>33470</v>
       </c>
-      <c r="C23" s="20"/>
+      <c r="C23" s="20">
+        <f>COUNTIFS(Reservas[Estado],A23,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
+        <v>4</v>
+      </c>
       <c r="D23" s="20"/>
       <c r="E23" s="24"/>
       <c r="F23" s="25"/>
@@ -22502,7 +22559,10 @@
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A24,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
         <v>0</v>
       </c>
-      <c r="C24" s="20"/>
+      <c r="C24" s="20">
+        <f>COUNTIFS(Reservas[Estado],A24,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
+        <v>0</v>
+      </c>
       <c r="D24" s="20"/>
       <c r="E24" s="24"/>
       <c r="F24" s="25"/>
@@ -22527,7 +22587,10 @@
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A25,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
         <v>0</v>
       </c>
-      <c r="C25" s="20"/>
+      <c r="C25" s="20">
+        <f>COUNTIFS(Reservas[Estado],A25,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
+        <v>0</v>
+      </c>
       <c r="D25" s="20"/>
       <c r="E25" s="24"/>
       <c r="F25" s="25"/>
@@ -22552,7 +22615,10 @@
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A26,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
         <v>0</v>
       </c>
-      <c r="C26" s="20"/>
+      <c r="C26" s="20">
+        <f>COUNTIFS(Reservas[Estado],A26,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
+        <v>0</v>
+      </c>
       <c r="D26" s="20"/>
       <c r="E26" s="24"/>
       <c r="F26" s="25"/>
@@ -22577,7 +22643,10 @@
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A27,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
         <v>0</v>
       </c>
-      <c r="C27" s="20"/>
+      <c r="C27" s="20">
+        <f>COUNTIFS(Reservas[Estado],A27,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
+        <v>0</v>
+      </c>
       <c r="D27" s="20"/>
       <c r="E27" s="24"/>
       <c r="F27" s="25"/>
@@ -22602,7 +22671,10 @@
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A28,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
         <v>0</v>
       </c>
-      <c r="C28" s="20"/>
+      <c r="C28" s="20">
+        <f>COUNTIFS(Reservas[Estado],A28,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
+        <v>0</v>
+      </c>
       <c r="D28" s="20"/>
       <c r="E28" s="24"/>
       <c r="F28" s="25"/>
@@ -22627,7 +22699,10 @@
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A29,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
         <v>36670</v>
       </c>
-      <c r="C29" s="20"/>
+      <c r="C29" s="20">
+        <f>COUNTIFS(Reservas[Estado],A29,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
+        <v>3</v>
+      </c>
       <c r="D29" s="20"/>
       <c r="E29" s="24"/>
       <c r="F29" s="25"/>
@@ -22648,7 +22723,10 @@
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A30,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
         <v>0</v>
       </c>
-      <c r="C30" s="20"/>
+      <c r="C30" s="20">
+        <f>COUNTIFS(Reservas[Estado],A30,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
+        <v>0</v>
+      </c>
       <c r="D30" s="20"/>
       <c r="E30" s="24"/>
       <c r="F30" s="25"/>
@@ -22673,7 +22751,10 @@
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A31,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
         <v>0</v>
       </c>
-      <c r="C31" s="20"/>
+      <c r="C31" s="20">
+        <f>COUNTIFS(Reservas[Estado],A31,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
+        <v>0</v>
+      </c>
       <c r="D31" s="20"/>
       <c r="E31" s="24"/>
       <c r="F31" s="25"/>

</xml_diff>

<commit_message>
Terminado de implementar contas para analises dos estados
</commit_message>
<xml_diff>
--- a/dashboards_II.xlsx
+++ b/dashboards_II.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c548d412d6f19400/Área de Trabalho/Alura/excel/Projetos Git/04. DashBoard Especialista/02.Dashboard 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{8621F33A-E581-4B2B-8C24-DD17DCFBD997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA7B101C-C721-467E-9FA7-C9F568E15A76}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="13_ncr:1_{8621F33A-E581-4B2B-8C24-DD17DCFBD997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF33491E-5E76-4C1A-B99F-E27B622AEAE3}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="3" xr2:uid="{18B12833-7551-4467-B611-A6E8F662E40B}"/>
   </bookViews>
@@ -818,7 +818,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="12" dropStyle="combo" dx="16" fmlaLink="Auxiliar!$L$5" fmlaRange="ListaMeses" sel="6" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="12" dropStyle="combo" dx="16" fmlaLink="Auxiliar!$L$5" fmlaRange="ListaMeses" sel="7" val="0"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -21968,7 +21968,7 @@
   <dimension ref="A1:S39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C31"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22075,9 +22075,18 @@
         <f>COUNTIFS(Reservas[Estado],A5,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
         <v>0</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="25"/>
+      <c r="D5" s="20">
+        <f>COUNTIFS(Reservas[Estado],A5,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="24" t="str">
+        <f>IFERROR(C5/D5,"0%")</f>
+        <v>0%</v>
+      </c>
+      <c r="F5" s="25">
+        <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A5,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
+        <v>0</v>
+      </c>
       <c r="H5" s="18" t="s">
         <v>55</v>
       </c>
@@ -22091,7 +22100,7 @@
         <v>2018</v>
       </c>
       <c r="L5" s="30">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -22100,15 +22109,24 @@
       </c>
       <c r="B6" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A6,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>0</v>
+        <v>1380</v>
       </c>
       <c r="C6" s="20">
         <f>COUNTIFS(Reservas[Estado],A6,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
         <v>0</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="25"/>
+      <c r="D6" s="20">
+        <f>COUNTIFS(Reservas[Estado],A6,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
+        <v>1</v>
+      </c>
+      <c r="E6" s="24">
+        <f t="shared" ref="E6:E31" si="0">IFERROR(C6/D6,"0%")</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="25">
+        <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A6,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
+        <v>5</v>
+      </c>
       <c r="H6" s="18" t="s">
         <v>56</v>
       </c>
@@ -22132,9 +22150,18 @@
         <f>COUNTIFS(Reservas[Estado],A7,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
         <v>0</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="25"/>
+      <c r="D7" s="20">
+        <f>COUNTIFS(Reservas[Estado],A7,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>0%</v>
+      </c>
+      <c r="F7" s="25">
+        <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A7,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="17" t="s">
@@ -22148,9 +22175,18 @@
         <f>COUNTIFS(Reservas[Estado],A8,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
         <v>0</v>
       </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="25"/>
+      <c r="D8" s="20">
+        <f>COUNTIFS(Reservas[Estado],A8,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>0%</v>
+      </c>
+      <c r="F8" s="25">
+        <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A8,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="17" t="s">
@@ -22164,9 +22200,18 @@
         <f>COUNTIFS(Reservas[Estado],A9,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
         <v>0</v>
       </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="25"/>
+      <c r="D9" s="20">
+        <f>COUNTIFS(Reservas[Estado],A9,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>0%</v>
+      </c>
+      <c r="F9" s="25">
+        <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A9,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
+        <v>0</v>
+      </c>
       <c r="H9" s="33" t="s">
         <v>58</v>
       </c>
@@ -22188,15 +22233,24 @@
       </c>
       <c r="B10" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A10,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>0</v>
+        <v>1415</v>
       </c>
       <c r="C10" s="20">
         <f>COUNTIFS(Reservas[Estado],A10,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>0</v>
-      </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="25"/>
+        <v>1</v>
+      </c>
+      <c r="D10" s="20">
+        <f>COUNTIFS(Reservas[Estado],A10,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
+        <v>1</v>
+      </c>
+      <c r="E10" s="24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F10" s="25">
+        <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A10,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
+        <v>5</v>
+      </c>
       <c r="H10" s="5" t="s">
         <v>59</v>
       </c>
@@ -22216,15 +22270,24 @@
       </c>
       <c r="B11" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A11,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>0</v>
+        <v>5800</v>
       </c>
       <c r="C11" s="20">
         <f>COUNTIFS(Reservas[Estado],A11,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
         <v>0</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="25"/>
+      <c r="D11" s="20">
+        <f>COUNTIFS(Reservas[Estado],A11,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
+        <v>2</v>
+      </c>
+      <c r="E11" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="25">
+        <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A11,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
+        <v>4.5</v>
+      </c>
       <c r="H11" s="19">
         <v>2018</v>
       </c>
@@ -22244,15 +22307,24 @@
       </c>
       <c r="B12" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A12,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>9880</v>
+        <v>3355</v>
       </c>
       <c r="C12" s="20">
         <f>COUNTIFS(Reservas[Estado],A12,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
+        <v>1</v>
+      </c>
+      <c r="D12" s="20">
+        <f>COUNTIFS(Reservas[Estado],A12,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
         <v>2</v>
       </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="25"/>
+      <c r="E12" s="24">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="F12" s="25">
+        <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A12,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
+        <v>5</v>
+      </c>
       <c r="H12" s="19">
         <v>2019</v>
       </c>
@@ -22272,15 +22344,24 @@
       </c>
       <c r="B13" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A13,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>3200</v>
+        <v>5335</v>
       </c>
       <c r="C13" s="20">
         <f>COUNTIFS(Reservas[Estado],A13,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>0</v>
-      </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="25"/>
+        <v>1</v>
+      </c>
+      <c r="D13" s="20">
+        <f>COUNTIFS(Reservas[Estado],A13,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
+        <v>3</v>
+      </c>
+      <c r="E13" s="24">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F13" s="25">
+        <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A13,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
+        <v>4.333333333333333</v>
+      </c>
       <c r="H13" s="19"/>
       <c r="I13" s="16" t="s">
         <v>63</v>
@@ -22298,15 +22379,24 @@
       </c>
       <c r="B14" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A14,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>0</v>
+        <v>1520</v>
       </c>
       <c r="C14" s="20">
         <f>COUNTIFS(Reservas[Estado],A14,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
         <v>0</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="25"/>
+      <c r="D14" s="20">
+        <f>COUNTIFS(Reservas[Estado],A14,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
+        <v>1</v>
+      </c>
+      <c r="E14" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="25">
+        <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A14,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
+        <v>5</v>
+      </c>
       <c r="H14" s="19"/>
       <c r="I14" s="16" t="s">
         <v>64</v>
@@ -22324,15 +22414,24 @@
       </c>
       <c r="B15" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A15,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>0</v>
+        <v>1555</v>
       </c>
       <c r="C15" s="20">
         <f>COUNTIFS(Reservas[Estado],A15,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
         <v>0</v>
       </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="25"/>
+      <c r="D15" s="20">
+        <f>COUNTIFS(Reservas[Estado],A15,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
+        <v>1</v>
+      </c>
+      <c r="E15" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="25">
+        <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A15,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
+        <v>5</v>
+      </c>
       <c r="H15" s="19"/>
       <c r="I15" s="16" t="s">
         <v>65</v>
@@ -22350,15 +22449,24 @@
       </c>
       <c r="B16" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A16,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>0</v>
+        <v>1590</v>
       </c>
       <c r="C16" s="20">
         <f>COUNTIFS(Reservas[Estado],A16,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>0</v>
-      </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="25"/>
+        <v>1</v>
+      </c>
+      <c r="D16" s="20">
+        <f>COUNTIFS(Reservas[Estado],A16,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
+        <v>1</v>
+      </c>
+      <c r="E16" s="24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F16" s="25">
+        <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A16,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
+        <v>4</v>
+      </c>
       <c r="H16" s="19"/>
       <c r="I16" s="16" t="s">
         <v>66</v>
@@ -22376,15 +22484,24 @@
       </c>
       <c r="B17" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A17,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>16455</v>
+        <v>5820</v>
       </c>
       <c r="C17" s="20">
         <f>COUNTIFS(Reservas[Estado],A17,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
         <v>2</v>
       </c>
-      <c r="D17" s="20"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="25"/>
+      <c r="D17" s="20">
+        <f>COUNTIFS(Reservas[Estado],A17,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
+        <v>3</v>
+      </c>
+      <c r="E17" s="24">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F17" s="25">
+        <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A17,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
+        <v>4.666666666666667</v>
+      </c>
       <c r="H17" s="19"/>
       <c r="I17" s="16" t="s">
         <v>67</v>
@@ -22402,15 +22519,24 @@
       </c>
       <c r="B18" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A18,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>0</v>
+        <v>1660</v>
       </c>
       <c r="C18" s="20">
         <f>COUNTIFS(Reservas[Estado],A18,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>0</v>
-      </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="25"/>
+        <v>1</v>
+      </c>
+      <c r="D18" s="20">
+        <f>COUNTIFS(Reservas[Estado],A18,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
+        <v>1</v>
+      </c>
+      <c r="E18" s="24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F18" s="25">
+        <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A18,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
+        <v>5</v>
+      </c>
       <c r="H18" s="19"/>
       <c r="I18" s="16" t="s">
         <v>68</v>
@@ -22428,15 +22554,24 @@
       </c>
       <c r="B19" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A19,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>0</v>
+        <v>1695</v>
       </c>
       <c r="C19" s="20">
         <f>COUNTIFS(Reservas[Estado],A19,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
         <v>0</v>
       </c>
-      <c r="D19" s="20"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="25"/>
+      <c r="D19" s="20">
+        <f>COUNTIFS(Reservas[Estado],A19,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
+        <v>1</v>
+      </c>
+      <c r="E19" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="25">
+        <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A19,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
+        <v>5</v>
+      </c>
       <c r="H19" s="19"/>
       <c r="I19" s="16" t="s">
         <v>69</v>
@@ -22454,15 +22589,24 @@
       </c>
       <c r="B20" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A20,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>0</v>
+        <v>1730</v>
       </c>
       <c r="C20" s="20">
         <f>COUNTIFS(Reservas[Estado],A20,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
         <v>0</v>
       </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="25"/>
+      <c r="D20" s="20">
+        <f>COUNTIFS(Reservas[Estado],A20,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
+        <v>1</v>
+      </c>
+      <c r="E20" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="25">
+        <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A20,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
+        <v>5</v>
+      </c>
       <c r="H20" s="19"/>
       <c r="I20" s="16" t="s">
         <v>70</v>
@@ -22474,15 +22618,24 @@
       </c>
       <c r="B21" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A21,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>0</v>
+        <v>8075</v>
       </c>
       <c r="C21" s="20">
         <f>COUNTIFS(Reservas[Estado],A21,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>0</v>
-      </c>
-      <c r="D21" s="20"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="25"/>
+        <v>2</v>
+      </c>
+      <c r="D21" s="20">
+        <f>COUNTIFS(Reservas[Estado],A21,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
+        <v>4</v>
+      </c>
+      <c r="E21" s="24">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="F21" s="25">
+        <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A21,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
+        <v>4.5</v>
+      </c>
       <c r="H21" s="19"/>
       <c r="I21" s="16" t="s">
         <v>71</v>
@@ -22501,15 +22654,24 @@
       </c>
       <c r="B22" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A22,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>0</v>
+        <v>1905</v>
       </c>
       <c r="C22" s="20">
         <f>COUNTIFS(Reservas[Estado],A22,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
         <v>0</v>
       </c>
-      <c r="D22" s="20"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="25"/>
+      <c r="D22" s="20">
+        <f>COUNTIFS(Reservas[Estado],A22,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
+        <v>1</v>
+      </c>
+      <c r="E22" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="25">
+        <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A22,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
+        <v>4</v>
+      </c>
       <c r="H22" s="19"/>
       <c r="I22" s="16" t="s">
         <v>72</v>
@@ -22533,15 +22695,24 @@
       </c>
       <c r="B23" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A23,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>33470</v>
+        <v>2345</v>
       </c>
       <c r="C23" s="20">
         <f>COUNTIFS(Reservas[Estado],A23,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>4</v>
-      </c>
-      <c r="D23" s="20"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="25"/>
+        <v>0</v>
+      </c>
+      <c r="D23" s="20">
+        <f>COUNTIFS(Reservas[Estado],A23,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
+        <v>1</v>
+      </c>
+      <c r="E23" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="25">
+        <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A23,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
+        <v>5</v>
+      </c>
       <c r="K23" s="26">
         <v>1</v>
       </c>
@@ -22557,15 +22728,24 @@
       </c>
       <c r="B24" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A24,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>0</v>
+        <v>1940</v>
       </c>
       <c r="C24" s="20">
         <f>COUNTIFS(Reservas[Estado],A24,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>0</v>
-      </c>
-      <c r="D24" s="20"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="25"/>
+        <v>1</v>
+      </c>
+      <c r="D24" s="20">
+        <f>COUNTIFS(Reservas[Estado],A24,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
+        <v>1</v>
+      </c>
+      <c r="E24" s="24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F24" s="25">
+        <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A24,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
+        <v>5</v>
+      </c>
       <c r="H24" s="33" t="s">
         <v>92</v>
       </c>
@@ -22585,15 +22765,24 @@
       </c>
       <c r="B25" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A25,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>0</v>
+        <v>1975</v>
       </c>
       <c r="C25" s="20">
         <f>COUNTIFS(Reservas[Estado],A25,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
         <v>0</v>
       </c>
-      <c r="D25" s="20"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="25"/>
+      <c r="D25" s="20">
+        <f>COUNTIFS(Reservas[Estado],A25,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
+        <v>1</v>
+      </c>
+      <c r="E25" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="25">
+        <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A25,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
+        <v>5</v>
+      </c>
       <c r="H25" s="27" t="s">
         <v>0</v>
       </c>
@@ -22613,15 +22802,24 @@
       </c>
       <c r="B26" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A26,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>0</v>
+        <v>2045</v>
       </c>
       <c r="C26" s="20">
         <f>COUNTIFS(Reservas[Estado],A26,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
         <v>0</v>
       </c>
-      <c r="D26" s="20"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="25"/>
+      <c r="D26" s="20">
+        <f>COUNTIFS(Reservas[Estado],A26,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
+        <v>1</v>
+      </c>
+      <c r="E26" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="25">
+        <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A26,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
+        <v>5</v>
+      </c>
       <c r="H26" s="27" t="s">
         <v>1</v>
       </c>
@@ -22641,15 +22839,24 @@
       </c>
       <c r="B27" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A27,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>0</v>
+        <v>2080</v>
       </c>
       <c r="C27" s="20">
         <f>COUNTIFS(Reservas[Estado],A27,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
         <v>0</v>
       </c>
-      <c r="D27" s="20"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="25"/>
+      <c r="D27" s="20">
+        <f>COUNTIFS(Reservas[Estado],A27,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
+        <v>1</v>
+      </c>
+      <c r="E27" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="25">
+        <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A27,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
+        <v>5</v>
+      </c>
       <c r="H27" s="27" t="s">
         <v>2</v>
       </c>
@@ -22669,15 +22876,24 @@
       </c>
       <c r="B28" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A28,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>0</v>
+        <v>2115</v>
       </c>
       <c r="C28" s="20">
         <f>COUNTIFS(Reservas[Estado],A28,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>0</v>
-      </c>
-      <c r="D28" s="20"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="25"/>
+        <v>1</v>
+      </c>
+      <c r="D28" s="20">
+        <f>COUNTIFS(Reservas[Estado],A28,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
+        <v>1</v>
+      </c>
+      <c r="E28" s="24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F28" s="25">
+        <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A28,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
+        <v>4</v>
+      </c>
       <c r="H28" s="27" t="s">
         <v>3</v>
       </c>
@@ -22697,15 +22913,24 @@
       </c>
       <c r="B29" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A29,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>36670</v>
+        <v>12213</v>
       </c>
       <c r="C29" s="20">
         <f>COUNTIFS(Reservas[Estado],A29,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>3</v>
-      </c>
-      <c r="D29" s="20"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="25"/>
+        <v>0</v>
+      </c>
+      <c r="D29" s="20">
+        <f>COUNTIFS(Reservas[Estado],A29,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
+        <v>4</v>
+      </c>
+      <c r="E29" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="25">
+        <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A29,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
+        <v>4.5</v>
+      </c>
       <c r="K29" s="26">
         <v>7</v>
       </c>
@@ -22721,15 +22946,24 @@
       </c>
       <c r="B30" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A30,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>0</v>
+        <v>2185</v>
       </c>
       <c r="C30" s="20">
         <f>COUNTIFS(Reservas[Estado],A30,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>0</v>
-      </c>
-      <c r="D30" s="20"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="25"/>
+        <v>1</v>
+      </c>
+      <c r="D30" s="20">
+        <f>COUNTIFS(Reservas[Estado],A30,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
+        <v>1</v>
+      </c>
+      <c r="E30" s="24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F30" s="25">
+        <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A30,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
+        <v>5</v>
+      </c>
       <c r="H30" s="33" t="s">
         <v>95</v>
       </c>
@@ -22749,15 +22983,24 @@
       </c>
       <c r="B31" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A31,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>0</v>
+        <v>2255</v>
       </c>
       <c r="C31" s="20">
         <f>COUNTIFS(Reservas[Estado],A31,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
         <v>0</v>
       </c>
-      <c r="D31" s="20"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="25"/>
+      <c r="D31" s="20">
+        <f>COUNTIFS(Reservas[Estado],A31,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
+        <v>1</v>
+      </c>
+      <c r="E31" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F31" s="25">
+        <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A31,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
+        <v>5</v>
+      </c>
       <c r="H31" s="27" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
implementando calculos do top 10
</commit_message>
<xml_diff>
--- a/dashboards_II.xlsx
+++ b/dashboards_II.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c548d412d6f19400/Área de Trabalho/Alura/excel/Projetos Git/04. DashBoard Especialista/02.Dashboard 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="13_ncr:1_{8621F33A-E581-4B2B-8C24-DD17DCFBD997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF33491E-5E76-4C1A-B99F-E27B622AEAE3}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:1_{8621F33A-E581-4B2B-8C24-DD17DCFBD997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14D717E4-EF5C-4A5F-9CAE-4E7FB048640E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="3" xr2:uid="{18B12833-7551-4467-B611-A6E8F662E40B}"/>
   </bookViews>
@@ -21967,8 +21967,8 @@
   </sheetPr>
   <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22261,7 +22261,10 @@
         <v>1</v>
       </c>
       <c r="L10" s="17"/>
-      <c r="M10" s="16"/>
+      <c r="M10" s="16">
+        <f>LARGE(Auxiliar!ListaVendas,K10)</f>
+        <v>12213</v>
+      </c>
       <c r="N10" s="24"/>
     </row>
     <row r="11" spans="1:19">
@@ -22298,7 +22301,10 @@
         <v>2</v>
       </c>
       <c r="L11" s="17"/>
-      <c r="M11" s="16"/>
+      <c r="M11" s="16">
+        <f>LARGE(Auxiliar!ListaVendas,K11)</f>
+        <v>8075</v>
+      </c>
       <c r="N11" s="24"/>
     </row>
     <row r="12" spans="1:19">
@@ -22335,7 +22341,10 @@
         <v>3</v>
       </c>
       <c r="L12" s="17"/>
-      <c r="M12" s="16"/>
+      <c r="M12" s="16">
+        <f>LARGE(Auxiliar!ListaVendas,K12)</f>
+        <v>5820</v>
+      </c>
       <c r="N12" s="24"/>
     </row>
     <row r="13" spans="1:19">
@@ -22370,7 +22379,10 @@
         <v>4</v>
       </c>
       <c r="L13" s="17"/>
-      <c r="M13" s="16"/>
+      <c r="M13" s="16">
+        <f>LARGE(Auxiliar!ListaVendas,K13)</f>
+        <v>5800</v>
+      </c>
       <c r="N13" s="24"/>
     </row>
     <row r="14" spans="1:19">
@@ -22405,7 +22417,10 @@
         <v>5</v>
       </c>
       <c r="L14" s="17"/>
-      <c r="M14" s="16"/>
+      <c r="M14" s="16">
+        <f>LARGE(Auxiliar!ListaVendas,K14)</f>
+        <v>5335</v>
+      </c>
       <c r="N14" s="24"/>
     </row>
     <row r="15" spans="1:19">
@@ -22440,7 +22455,10 @@
         <v>6</v>
       </c>
       <c r="L15" s="17"/>
-      <c r="M15" s="16"/>
+      <c r="M15" s="16">
+        <f>LARGE(Auxiliar!ListaVendas,K15)</f>
+        <v>3355</v>
+      </c>
       <c r="N15" s="24"/>
     </row>
     <row r="16" spans="1:19">
@@ -22475,7 +22493,10 @@
         <v>7</v>
       </c>
       <c r="L16" s="17"/>
-      <c r="M16" s="16"/>
+      <c r="M16" s="16">
+        <f>LARGE(Auxiliar!ListaVendas,K16)</f>
+        <v>2345</v>
+      </c>
       <c r="N16" s="24"/>
     </row>
     <row r="17" spans="1:14">
@@ -22510,7 +22531,10 @@
         <v>8</v>
       </c>
       <c r="L17" s="17"/>
-      <c r="M17" s="16"/>
+      <c r="M17" s="16">
+        <f>LARGE(Auxiliar!ListaVendas,K17)</f>
+        <v>2255</v>
+      </c>
       <c r="N17" s="24"/>
     </row>
     <row r="18" spans="1:14">
@@ -22545,7 +22569,10 @@
         <v>9</v>
       </c>
       <c r="L18" s="17"/>
-      <c r="M18" s="16"/>
+      <c r="M18" s="16">
+        <f>LARGE(Auxiliar!ListaVendas,K18)</f>
+        <v>2185</v>
+      </c>
       <c r="N18" s="24"/>
     </row>
     <row r="19" spans="1:14">
@@ -22580,7 +22607,10 @@
         <v>10</v>
       </c>
       <c r="L19" s="17"/>
-      <c r="M19" s="16"/>
+      <c r="M19" s="16">
+        <f>LARGE(Auxiliar!ListaVendas,K19)</f>
+        <v>2115</v>
+      </c>
       <c r="N19" s="24"/>
     </row>
     <row r="20" spans="1:14">

</xml_diff>

<commit_message>
Implementando calculos dos top estados
</commit_message>
<xml_diff>
--- a/dashboards_II.xlsx
+++ b/dashboards_II.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c548d412d6f19400/Área de Trabalho/Alura/excel/Projetos Git/04. DashBoard Especialista/02.Dashboard 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:1_{8621F33A-E581-4B2B-8C24-DD17DCFBD997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14D717E4-EF5C-4A5F-9CAE-4E7FB048640E}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="13_ncr:1_{8621F33A-E581-4B2B-8C24-DD17DCFBD997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9333813-1EC8-4F97-B39E-E550F8C7D60C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="3" xr2:uid="{18B12833-7551-4467-B611-A6E8F662E40B}"/>
   </bookViews>
@@ -810,7 +810,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="16" fmlaLink="Auxiliar!$I$6" fmlaRange="ListaEstados" sel="5" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="16" fmlaLink="Auxiliar!$I$6" fmlaRange="ListaEstados" sel="25" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -818,7 +818,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="12" dropStyle="combo" dx="16" fmlaLink="Auxiliar!$L$5" fmlaRange="ListaMeses" sel="7" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="12" dropStyle="combo" dx="16" fmlaLink="Auxiliar!$L$5" fmlaRange="ListaMeses" sel="8" val="0"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -22092,7 +22092,7 @@
       </c>
       <c r="I5" s="35" t="str" cm="1">
         <f t="array" ref="I5">INDEX(Auxiliar!ListaEstados,Auxiliar!IndiceEstado)</f>
-        <v>Bahia</v>
+        <v>São Paulo</v>
       </c>
       <c r="J5" s="36"/>
       <c r="K5" s="23" cm="1">
@@ -22100,7 +22100,7 @@
         <v>2018</v>
       </c>
       <c r="L5" s="30">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -22109,7 +22109,7 @@
       </c>
       <c r="B6" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A6,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>1380</v>
+        <v>0</v>
       </c>
       <c r="C6" s="20">
         <f>COUNTIFS(Reservas[Estado],A6,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
@@ -22117,21 +22117,21 @@
       </c>
       <c r="D6" s="20">
         <f>COUNTIFS(Reservas[Estado],A6,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>1</v>
-      </c>
-      <c r="E6" s="24">
+        <v>0</v>
+      </c>
+      <c r="E6" s="24" t="str">
         <f t="shared" ref="E6:E31" si="0">IFERROR(C6/D6,"0%")</f>
-        <v>0</v>
+        <v>0%</v>
       </c>
       <c r="F6" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A6,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H6" s="18" t="s">
         <v>56</v>
       </c>
       <c r="I6" s="37">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="J6" s="37"/>
       <c r="K6" s="30">
@@ -22233,23 +22233,23 @@
       </c>
       <c r="B10" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A10,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>1415</v>
+        <v>0</v>
       </c>
       <c r="C10" s="20">
         <f>COUNTIFS(Reservas[Estado],A10,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" s="20">
         <f>COUNTIFS(Reservas[Estado],A10,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>1</v>
-      </c>
-      <c r="E10" s="24">
+        <v>0</v>
+      </c>
+      <c r="E10" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0%</v>
       </c>
       <c r="F10" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A10,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>59</v>
@@ -22260,10 +22260,13 @@
       <c r="K10" s="26">
         <v>1</v>
       </c>
-      <c r="L10" s="17"/>
+      <c r="L10" s="17" t="str">
+        <f>IF(M10&gt;0,INDEX(Auxiliar!ListaEstados,MATCH(M10,Auxiliar!ListaVendas,0)),"")</f>
+        <v>São Paulo</v>
+      </c>
       <c r="M10" s="16">
         <f>LARGE(Auxiliar!ListaVendas,K10)</f>
-        <v>12213</v>
+        <v>26315</v>
       </c>
       <c r="N10" s="24"/>
     </row>
@@ -22273,23 +22276,23 @@
       </c>
       <c r="B11" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A11,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>5800</v>
+        <v>2640</v>
       </c>
       <c r="C11" s="20">
         <f>COUNTIFS(Reservas[Estado],A11,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="20">
         <f>COUNTIFS(Reservas[Estado],A11,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A11,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="H11" s="19">
         <v>2018</v>
@@ -22300,10 +22303,13 @@
       <c r="K11" s="26">
         <v>2</v>
       </c>
-      <c r="L11" s="17"/>
+      <c r="L11" s="17" t="str">
+        <f>IF(M11&gt;0,INDEX(Auxiliar!ListaEstados,MATCH(M11,Auxiliar!ListaVendas,0)),"")</f>
+        <v>Rio de Janeiro</v>
+      </c>
       <c r="M11" s="16">
         <f>LARGE(Auxiliar!ListaVendas,K11)</f>
-        <v>8075</v>
+        <v>26160</v>
       </c>
       <c r="N11" s="24"/>
     </row>
@@ -22313,23 +22319,23 @@
       </c>
       <c r="B12" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A12,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>3355</v>
+        <v>8620</v>
       </c>
       <c r="C12" s="20">
         <f>COUNTIFS(Reservas[Estado],A12,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="20">
         <f>COUNTIFS(Reservas[Estado],A12,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E12" s="24">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F12" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A12,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H12" s="19">
         <v>2019</v>
@@ -22340,10 +22346,13 @@
       <c r="K12" s="26">
         <v>3</v>
       </c>
-      <c r="L12" s="17"/>
+      <c r="L12" s="17" t="str">
+        <f>IF(M12&gt;0,INDEX(Auxiliar!ListaEstados,MATCH(M12,Auxiliar!ListaVendas,0)),"")</f>
+        <v>Minas Gerais</v>
+      </c>
       <c r="M12" s="16">
         <f>LARGE(Auxiliar!ListaVendas,K12)</f>
-        <v>5820</v>
+        <v>17918</v>
       </c>
       <c r="N12" s="24"/>
     </row>
@@ -22353,23 +22362,23 @@
       </c>
       <c r="B13" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A13,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>5335</v>
+        <v>0</v>
       </c>
       <c r="C13" s="20">
         <f>COUNTIFS(Reservas[Estado],A13,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" s="20">
         <f>COUNTIFS(Reservas[Estado],A13,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>3</v>
-      </c>
-      <c r="E13" s="24">
+        <v>0</v>
+      </c>
+      <c r="E13" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0%</v>
       </c>
       <c r="F13" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A13,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>4.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="H13" s="19"/>
       <c r="I13" s="16" t="s">
@@ -22378,10 +22387,13 @@
       <c r="K13" s="26">
         <v>4</v>
       </c>
-      <c r="L13" s="17"/>
+      <c r="L13" s="17" t="str">
+        <f>IF(M13&gt;0,INDEX(Auxiliar!ListaEstados,MATCH(M13,Auxiliar!ListaVendas,0)),"")</f>
+        <v>Espírito Santo</v>
+      </c>
       <c r="M13" s="16">
         <f>LARGE(Auxiliar!ListaVendas,K13)</f>
-        <v>5800</v>
+        <v>8620</v>
       </c>
       <c r="N13" s="24"/>
     </row>
@@ -22391,7 +22403,7 @@
       </c>
       <c r="B14" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A14,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>1520</v>
+        <v>0</v>
       </c>
       <c r="C14" s="20">
         <f>COUNTIFS(Reservas[Estado],A14,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
@@ -22399,15 +22411,15 @@
       </c>
       <c r="D14" s="20">
         <f>COUNTIFS(Reservas[Estado],A14,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>1</v>
-      </c>
-      <c r="E14" s="24">
+        <v>0</v>
+      </c>
+      <c r="E14" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0%</v>
       </c>
       <c r="F14" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A14,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H14" s="19"/>
       <c r="I14" s="16" t="s">
@@ -22416,10 +22428,13 @@
       <c r="K14" s="26">
         <v>5</v>
       </c>
-      <c r="L14" s="17"/>
+      <c r="L14" s="17" t="str">
+        <f>IF(M14&gt;0,INDEX(Auxiliar!ListaEstados,MATCH(M14,Auxiliar!ListaVendas,0)),"")</f>
+        <v>Rio Grande do Sul</v>
+      </c>
       <c r="M14" s="16">
         <f>LARGE(Auxiliar!ListaVendas,K14)</f>
-        <v>5335</v>
+        <v>5105</v>
       </c>
       <c r="N14" s="24"/>
     </row>
@@ -22429,7 +22444,7 @@
       </c>
       <c r="B15" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A15,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>1555</v>
+        <v>0</v>
       </c>
       <c r="C15" s="20">
         <f>COUNTIFS(Reservas[Estado],A15,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
@@ -22437,15 +22452,15 @@
       </c>
       <c r="D15" s="20">
         <f>COUNTIFS(Reservas[Estado],A15,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>1</v>
-      </c>
-      <c r="E15" s="24">
+        <v>0</v>
+      </c>
+      <c r="E15" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0%</v>
       </c>
       <c r="F15" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A15,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="16" t="s">
@@ -22454,10 +22469,13 @@
       <c r="K15" s="26">
         <v>6</v>
       </c>
-      <c r="L15" s="17"/>
+      <c r="L15" s="17" t="str">
+        <f>IF(M15&gt;0,INDEX(Auxiliar!ListaEstados,MATCH(M15,Auxiliar!ListaVendas,0)),"")</f>
+        <v>Distrito Federal</v>
+      </c>
       <c r="M15" s="16">
         <f>LARGE(Auxiliar!ListaVendas,K15)</f>
-        <v>3355</v>
+        <v>2640</v>
       </c>
       <c r="N15" s="24"/>
     </row>
@@ -22467,23 +22485,23 @@
       </c>
       <c r="B16" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A16,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>1590</v>
+        <v>0</v>
       </c>
       <c r="C16" s="20">
         <f>COUNTIFS(Reservas[Estado],A16,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" s="20">
         <f>COUNTIFS(Reservas[Estado],A16,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>1</v>
-      </c>
-      <c r="E16" s="24">
+        <v>0</v>
+      </c>
+      <c r="E16" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0%</v>
       </c>
       <c r="F16" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A16,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="16" t="s">
@@ -22492,10 +22510,13 @@
       <c r="K16" s="26">
         <v>7</v>
       </c>
-      <c r="L16" s="17"/>
+      <c r="L16" s="17" t="str">
+        <f>IF(M16&gt;0,INDEX(Auxiliar!ListaEstados,MATCH(M16,Auxiliar!ListaVendas,0)),"")</f>
+        <v>Santa Catarina</v>
+      </c>
       <c r="M16" s="16">
         <f>LARGE(Auxiliar!ListaVendas,K16)</f>
-        <v>2345</v>
+        <v>2535</v>
       </c>
       <c r="N16" s="24"/>
     </row>
@@ -22505,23 +22526,23 @@
       </c>
       <c r="B17" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A17,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>5820</v>
+        <v>17918</v>
       </c>
       <c r="C17" s="20">
         <f>COUNTIFS(Reservas[Estado],A17,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17" s="20">
         <f>COUNTIFS(Reservas[Estado],A17,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E17" s="24">
         <f t="shared" si="0"/>
-        <v>0.66666666666666663</v>
+        <v>0.2</v>
       </c>
       <c r="F17" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A17,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>4.666666666666667</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="16" t="s">
@@ -22530,10 +22551,13 @@
       <c r="K17" s="26">
         <v>8</v>
       </c>
-      <c r="L17" s="17"/>
+      <c r="L17" s="17" t="str">
+        <f>IF(M17&gt;0,INDEX(Auxiliar!ListaEstados,MATCH(M17,Auxiliar!ListaVendas,0)),"")</f>
+        <v/>
+      </c>
       <c r="M17" s="16">
         <f>LARGE(Auxiliar!ListaVendas,K17)</f>
-        <v>2255</v>
+        <v>0</v>
       </c>
       <c r="N17" s="24"/>
     </row>
@@ -22543,23 +22567,23 @@
       </c>
       <c r="B18" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A18,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>1660</v>
+        <v>0</v>
       </c>
       <c r="C18" s="20">
         <f>COUNTIFS(Reservas[Estado],A18,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" s="20">
         <f>COUNTIFS(Reservas[Estado],A18,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>1</v>
-      </c>
-      <c r="E18" s="24">
+        <v>0</v>
+      </c>
+      <c r="E18" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0%</v>
       </c>
       <c r="F18" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A18,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="16" t="s">
@@ -22568,10 +22592,13 @@
       <c r="K18" s="26">
         <v>9</v>
       </c>
-      <c r="L18" s="17"/>
+      <c r="L18" s="17" t="str">
+        <f>IF(M18&gt;0,INDEX(Auxiliar!ListaEstados,MATCH(M18,Auxiliar!ListaVendas,0)),"")</f>
+        <v/>
+      </c>
       <c r="M18" s="16">
         <f>LARGE(Auxiliar!ListaVendas,K18)</f>
-        <v>2185</v>
+        <v>0</v>
       </c>
       <c r="N18" s="24"/>
     </row>
@@ -22581,7 +22608,7 @@
       </c>
       <c r="B19" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A19,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>1695</v>
+        <v>0</v>
       </c>
       <c r="C19" s="20">
         <f>COUNTIFS(Reservas[Estado],A19,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
@@ -22589,15 +22616,15 @@
       </c>
       <c r="D19" s="20">
         <f>COUNTIFS(Reservas[Estado],A19,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>1</v>
-      </c>
-      <c r="E19" s="24">
+        <v>0</v>
+      </c>
+      <c r="E19" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0%</v>
       </c>
       <c r="F19" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A19,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H19" s="19"/>
       <c r="I19" s="16" t="s">
@@ -22606,10 +22633,13 @@
       <c r="K19" s="26">
         <v>10</v>
       </c>
-      <c r="L19" s="17"/>
+      <c r="L19" s="17" t="str">
+        <f>IF(M19&gt;0,INDEX(Auxiliar!ListaEstados,MATCH(M19,Auxiliar!ListaVendas,0)),"")</f>
+        <v/>
+      </c>
       <c r="M19" s="16">
         <f>LARGE(Auxiliar!ListaVendas,K19)</f>
-        <v>2115</v>
+        <v>0</v>
       </c>
       <c r="N19" s="24"/>
     </row>
@@ -22619,7 +22649,7 @@
       </c>
       <c r="B20" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A20,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>1730</v>
+        <v>0</v>
       </c>
       <c r="C20" s="20">
         <f>COUNTIFS(Reservas[Estado],A20,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
@@ -22627,15 +22657,15 @@
       </c>
       <c r="D20" s="20">
         <f>COUNTIFS(Reservas[Estado],A20,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>1</v>
-      </c>
-      <c r="E20" s="24">
+        <v>0</v>
+      </c>
+      <c r="E20" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0%</v>
       </c>
       <c r="F20" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A20,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H20" s="19"/>
       <c r="I20" s="16" t="s">
@@ -22648,23 +22678,23 @@
       </c>
       <c r="B21" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A21,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>8075</v>
+        <v>0</v>
       </c>
       <c r="C21" s="20">
         <f>COUNTIFS(Reservas[Estado],A21,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D21" s="20">
         <f>COUNTIFS(Reservas[Estado],A21,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>4</v>
-      </c>
-      <c r="E21" s="24">
+        <v>0</v>
+      </c>
+      <c r="E21" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0%</v>
       </c>
       <c r="F21" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A21,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="H21" s="19"/>
       <c r="I21" s="16" t="s">
@@ -22672,7 +22702,7 @@
       </c>
       <c r="K21" s="33" t="str">
         <f>"Análise de Vendas "&amp;Estado</f>
-        <v>Análise de Vendas Bahia</v>
+        <v>Análise de Vendas São Paulo</v>
       </c>
       <c r="L21" s="33"/>
       <c r="M21" s="33"/>
@@ -22684,7 +22714,7 @@
       </c>
       <c r="B22" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A22,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>1905</v>
+        <v>0</v>
       </c>
       <c r="C22" s="20">
         <f>COUNTIFS(Reservas[Estado],A22,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
@@ -22692,15 +22722,15 @@
       </c>
       <c r="D22" s="20">
         <f>COUNTIFS(Reservas[Estado],A22,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>1</v>
-      </c>
-      <c r="E22" s="24">
+        <v>0</v>
+      </c>
+      <c r="E22" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0%</v>
       </c>
       <c r="F22" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A22,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H22" s="19"/>
       <c r="I22" s="16" t="s">
@@ -22725,23 +22755,23 @@
       </c>
       <c r="B23" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A23,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>2345</v>
+        <v>26160</v>
       </c>
       <c r="C23" s="20">
         <f>COUNTIFS(Reservas[Estado],A23,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D23" s="20">
         <f>COUNTIFS(Reservas[Estado],A23,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E23" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="F23" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A23,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>5</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="K23" s="26">
         <v>1</v>
@@ -22758,23 +22788,23 @@
       </c>
       <c r="B24" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A24,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>1940</v>
+        <v>0</v>
       </c>
       <c r="C24" s="20">
         <f>COUNTIFS(Reservas[Estado],A24,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" s="20">
         <f>COUNTIFS(Reservas[Estado],A24,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>1</v>
-      </c>
-      <c r="E24" s="24">
+        <v>0</v>
+      </c>
+      <c r="E24" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0%</v>
       </c>
       <c r="F24" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A24,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H24" s="33" t="s">
         <v>92</v>
@@ -22795,7 +22825,7 @@
       </c>
       <c r="B25" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A25,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>1975</v>
+        <v>5105</v>
       </c>
       <c r="C25" s="20">
         <f>COUNTIFS(Reservas[Estado],A25,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
@@ -22803,7 +22833,7 @@
       </c>
       <c r="D25" s="20">
         <f>COUNTIFS(Reservas[Estado],A25,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E25" s="24">
         <f t="shared" si="0"/>
@@ -22832,7 +22862,7 @@
       </c>
       <c r="B26" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A26,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>2045</v>
+        <v>0</v>
       </c>
       <c r="C26" s="20">
         <f>COUNTIFS(Reservas[Estado],A26,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
@@ -22840,15 +22870,15 @@
       </c>
       <c r="D26" s="20">
         <f>COUNTIFS(Reservas[Estado],A26,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>1</v>
-      </c>
-      <c r="E26" s="24">
+        <v>0</v>
+      </c>
+      <c r="E26" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0%</v>
       </c>
       <c r="F26" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A26,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H26" s="27" t="s">
         <v>1</v>
@@ -22869,7 +22899,7 @@
       </c>
       <c r="B27" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A27,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>2080</v>
+        <v>0</v>
       </c>
       <c r="C27" s="20">
         <f>COUNTIFS(Reservas[Estado],A27,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
@@ -22877,15 +22907,15 @@
       </c>
       <c r="D27" s="20">
         <f>COUNTIFS(Reservas[Estado],A27,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>1</v>
-      </c>
-      <c r="E27" s="24">
+        <v>0</v>
+      </c>
+      <c r="E27" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0%</v>
       </c>
       <c r="F27" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A27,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H27" s="27" t="s">
         <v>2</v>
@@ -22906,7 +22936,7 @@
       </c>
       <c r="B28" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A28,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>2115</v>
+        <v>2535</v>
       </c>
       <c r="C28" s="20">
         <f>COUNTIFS(Reservas[Estado],A28,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
@@ -22922,7 +22952,7 @@
       </c>
       <c r="F28" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A28,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H28" s="27" t="s">
         <v>3</v>
@@ -22943,23 +22973,23 @@
       </c>
       <c r="B29" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A29,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>12213</v>
+        <v>26315</v>
       </c>
       <c r="C29" s="20">
         <f>COUNTIFS(Reservas[Estado],A29,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D29" s="20">
         <f>COUNTIFS(Reservas[Estado],A29,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E29" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="F29" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A29,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>4.5</v>
+        <v>4.333333333333333</v>
       </c>
       <c r="K29" s="26">
         <v>7</v>
@@ -22976,23 +23006,23 @@
       </c>
       <c r="B30" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A30,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>2185</v>
+        <v>0</v>
       </c>
       <c r="C30" s="20">
         <f>COUNTIFS(Reservas[Estado],A30,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30" s="20">
         <f>COUNTIFS(Reservas[Estado],A30,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>1</v>
-      </c>
-      <c r="E30" s="24">
+        <v>0</v>
+      </c>
+      <c r="E30" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0%</v>
       </c>
       <c r="F30" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A30,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H30" s="33" t="s">
         <v>95</v>
@@ -23013,7 +23043,7 @@
       </c>
       <c r="B31" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A31,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>2255</v>
+        <v>0</v>
       </c>
       <c r="C31" s="20">
         <f>COUNTIFS(Reservas[Estado],A31,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
@@ -23021,15 +23051,15 @@
       </c>
       <c r="D31" s="20">
         <f>COUNTIFS(Reservas[Estado],A31,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>1</v>
-      </c>
-      <c r="E31" s="24">
+        <v>0</v>
+      </c>
+      <c r="E31" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0%</v>
       </c>
       <c r="F31" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A31,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H31" s="27" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Terminando de implementar calculos dos estados e implementando graficos
</commit_message>
<xml_diff>
--- a/dashboards_II.xlsx
+++ b/dashboards_II.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c548d412d6f19400/Área de Trabalho/Alura/excel/Projetos Git/04. DashBoard Especialista/02.Dashboard 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="78" documentId="13_ncr:1_{8621F33A-E581-4B2B-8C24-DD17DCFBD997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9333813-1EC8-4F97-B39E-E550F8C7D60C}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="13_ncr:1_{8621F33A-E581-4B2B-8C24-DD17DCFBD997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C8A0B96-FBE7-4EF5-981A-48572FA5E545}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="3" xr2:uid="{18B12833-7551-4467-B611-A6E8F662E40B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="4" xr2:uid="{18B12833-7551-4467-B611-A6E8F662E40B}"/>
   </bookViews>
   <sheets>
     <sheet name="Rascunho Dash" sheetId="15" state="hidden" r:id="rId1"/>
@@ -25,6 +25,8 @@
     <externalReference r:id="rId8"/>
   </externalReferences>
   <definedNames>
+    <definedName name="_xlchart.v2.0" hidden="1">Auxiliar!$L$10:$L$19</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">Auxiliar!$M$10:$M$19</definedName>
     <definedName name="Ano" localSheetId="3">Auxiliar!$K$5</definedName>
     <definedName name="Ano" localSheetId="4">Auxiliar!$K$5</definedName>
     <definedName name="Ano" localSheetId="0">Auxiliar!$K$5</definedName>
@@ -809,8 +811,615 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v2.0</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v2.1</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>10 Principais Estados Vendas</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>10 Principais Estados Vendas</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="funnel" uniqueId="{0CE54EC0-5959-429E-8085-5EC98614EF17}">
+          <cx:dataLabels>
+            <cx:visibility seriesName="0" categoryName="0" value="1"/>
+          </cx:dataLabels>
+          <cx:dataId val="0"/>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0.0599999987"/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="419">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="16" fmlaLink="Auxiliar!$I$6" fmlaRange="ListaEstados" sel="25" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="16" fmlaLink="Auxiliar!$I$6" fmlaRange="ListaEstados" sel="5" val="3"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -818,7 +1427,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="12" dropStyle="combo" dx="16" fmlaLink="Auxiliar!$L$5" fmlaRange="ListaMeses" sel="8" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="12" dropStyle="combo" dx="16" fmlaLink="Auxiliar!$L$5" fmlaRange="ListaMeses" sel="3" val="0"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1576,6 +2185,84 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>39220</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>43702</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>204508</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx2="http://schemas.microsoft.com/office/drawing/2015/10/21/chartex" Requires="cx2">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Gráfico 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F307CD2F-5895-68C9-DCA5-0C603B1F512A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="648820" y="558052"/>
+              <a:ext cx="3213288" cy="1927973"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100"/>
+                <a:t>Este gráfico não está disponível na sua versão de Excel.
+Editar esta forma ou salvar esta pasta de trabalho em um formato de arquivo diferente quebrará o gráfico permanentemente.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -21967,8 +22654,8 @@
   </sheetPr>
   <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -21985,7 +22672,8 @@
     <col min="10" max="10" width="3.7109375" customWidth="1"/>
     <col min="11" max="11" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12.7109375" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="3.7109375" customWidth="1"/>
     <col min="16" max="16" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="4.7109375" bestFit="1" customWidth="1"/>
@@ -22092,7 +22780,7 @@
       </c>
       <c r="I5" s="35" t="str" cm="1">
         <f t="array" ref="I5">INDEX(Auxiliar!ListaEstados,Auxiliar!IndiceEstado)</f>
-        <v>São Paulo</v>
+        <v>Bahia</v>
       </c>
       <c r="J5" s="36"/>
       <c r="K5" s="23" cm="1">
@@ -22100,7 +22788,7 @@
         <v>2018</v>
       </c>
       <c r="L5" s="30">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -22131,7 +22819,7 @@
         <v>56</v>
       </c>
       <c r="I6" s="37">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="J6" s="37"/>
       <c r="K6" s="30">
@@ -22262,13 +22950,16 @@
       </c>
       <c r="L10" s="17" t="str">
         <f>IF(M10&gt;0,INDEX(Auxiliar!ListaEstados,MATCH(M10,Auxiliar!ListaVendas,0)),"")</f>
-        <v>São Paulo</v>
+        <v>Pernambuco</v>
       </c>
       <c r="M10" s="16">
         <f>LARGE(Auxiliar!ListaVendas,K10)</f>
-        <v>26315</v>
-      </c>
-      <c r="N10" s="24"/>
+        <v>21340</v>
+      </c>
+      <c r="N10" s="24">
+        <f>IFERROR(VLOOKUP(L10,$A$4:$F$31,5,0),"0%")</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="17" t="s">
@@ -22276,7 +22967,7 @@
       </c>
       <c r="B11" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A11,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>2640</v>
+        <v>4055</v>
       </c>
       <c r="C11" s="20">
         <f>COUNTIFS(Reservas[Estado],A11,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
@@ -22284,15 +22975,15 @@
       </c>
       <c r="D11" s="20">
         <f>COUNTIFS(Reservas[Estado],A11,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" s="24">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F11" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A11,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H11" s="19">
         <v>2018</v>
@@ -22305,13 +22996,16 @@
       </c>
       <c r="L11" s="17" t="str">
         <f>IF(M11&gt;0,INDEX(Auxiliar!ListaEstados,MATCH(M11,Auxiliar!ListaVendas,0)),"")</f>
-        <v>Rio de Janeiro</v>
+        <v>São Paulo</v>
       </c>
       <c r="M11" s="16">
         <f>LARGE(Auxiliar!ListaVendas,K11)</f>
-        <v>26160</v>
-      </c>
-      <c r="N11" s="24"/>
+        <v>20857</v>
+      </c>
+      <c r="N11" s="24">
+        <f t="shared" ref="N11:N19" si="1">IFERROR(VLOOKUP(L11,$A$4:$F$31,5,0),"0%")</f>
+        <v>0.33333333333333331</v>
+      </c>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="17" t="s">
@@ -22319,7 +23013,7 @@
       </c>
       <c r="B12" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A12,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>8620</v>
+        <v>11682</v>
       </c>
       <c r="C12" s="20">
         <f>COUNTIFS(Reservas[Estado],A12,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
@@ -22327,7 +23021,7 @@
       </c>
       <c r="D12" s="20">
         <f>COUNTIFS(Reservas[Estado],A12,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E12" s="24">
         <f t="shared" si="0"/>
@@ -22335,7 +23029,7 @@
       </c>
       <c r="F12" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A12,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H12" s="19">
         <v>2019</v>
@@ -22348,13 +23042,16 @@
       </c>
       <c r="L12" s="17" t="str">
         <f>IF(M12&gt;0,INDEX(Auxiliar!ListaEstados,MATCH(M12,Auxiliar!ListaVendas,0)),"")</f>
-        <v>Minas Gerais</v>
+        <v>Espírito Santo</v>
       </c>
       <c r="M12" s="16">
         <f>LARGE(Auxiliar!ListaVendas,K12)</f>
-        <v>17918</v>
-      </c>
-      <c r="N12" s="24"/>
+        <v>11682</v>
+      </c>
+      <c r="N12" s="24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="17" t="s">
@@ -22389,13 +23086,16 @@
       </c>
       <c r="L13" s="17" t="str">
         <f>IF(M13&gt;0,INDEX(Auxiliar!ListaEstados,MATCH(M13,Auxiliar!ListaVendas,0)),"")</f>
-        <v>Espírito Santo</v>
+        <v>Santa Catarina</v>
       </c>
       <c r="M13" s="16">
         <f>LARGE(Auxiliar!ListaVendas,K13)</f>
-        <v>8620</v>
-      </c>
-      <c r="N13" s="24"/>
+        <v>11536</v>
+      </c>
+      <c r="N13" s="24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:19">
       <c r="A14" s="17" t="s">
@@ -22430,13 +23130,16 @@
       </c>
       <c r="L14" s="17" t="str">
         <f>IF(M14&gt;0,INDEX(Auxiliar!ListaEstados,MATCH(M14,Auxiliar!ListaVendas,0)),"")</f>
-        <v>Rio Grande do Sul</v>
+        <v>Minas Gerais</v>
       </c>
       <c r="M14" s="16">
         <f>LARGE(Auxiliar!ListaVendas,K14)</f>
-        <v>5105</v>
-      </c>
-      <c r="N14" s="24"/>
+        <v>9350</v>
+      </c>
+      <c r="N14" s="24">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
+      </c>
     </row>
     <row r="15" spans="1:19">
       <c r="A15" s="17" t="s">
@@ -22444,23 +23147,23 @@
       </c>
       <c r="B15" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A15,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>0</v>
+        <v>1345</v>
       </c>
       <c r="C15" s="20">
         <f>COUNTIFS(Reservas[Estado],A15,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="20">
         <f>COUNTIFS(Reservas[Estado],A15,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>0</v>
-      </c>
-      <c r="E15" s="24" t="str">
+        <v>1</v>
+      </c>
+      <c r="E15" s="24">
         <f t="shared" si="0"/>
-        <v>0%</v>
+        <v>1</v>
       </c>
       <c r="F15" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A15,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="16" t="s">
@@ -22471,13 +23174,16 @@
       </c>
       <c r="L15" s="17" t="str">
         <f>IF(M15&gt;0,INDEX(Auxiliar!ListaEstados,MATCH(M15,Auxiliar!ListaVendas,0)),"")</f>
-        <v>Distrito Federal</v>
+        <v>Roraima</v>
       </c>
       <c r="M15" s="16">
         <f>LARGE(Auxiliar!ListaVendas,K15)</f>
-        <v>2640</v>
-      </c>
-      <c r="N15" s="24"/>
+        <v>8765</v>
+      </c>
+      <c r="N15" s="24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="17" t="s">
@@ -22485,7 +23191,7 @@
       </c>
       <c r="B16" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A16,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>0</v>
+        <v>1380</v>
       </c>
       <c r="C16" s="20">
         <f>COUNTIFS(Reservas[Estado],A16,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
@@ -22493,15 +23199,15 @@
       </c>
       <c r="D16" s="20">
         <f>COUNTIFS(Reservas[Estado],A16,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
+        <v>1</v>
+      </c>
+      <c r="E16" s="24">
+        <f t="shared" si="0"/>
         <v>0</v>
-      </c>
-      <c r="E16" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>0%</v>
       </c>
       <c r="F16" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A16,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="16" t="s">
@@ -22512,13 +23218,16 @@
       </c>
       <c r="L16" s="17" t="str">
         <f>IF(M16&gt;0,INDEX(Auxiliar!ListaEstados,MATCH(M16,Auxiliar!ListaVendas,0)),"")</f>
-        <v>Santa Catarina</v>
+        <v>Rio Grande do Sul</v>
       </c>
       <c r="M16" s="16">
         <f>LARGE(Auxiliar!ListaVendas,K16)</f>
-        <v>2535</v>
-      </c>
-      <c r="N16" s="24"/>
+        <v>5890</v>
+      </c>
+      <c r="N16" s="24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:14">
       <c r="A17" s="17" t="s">
@@ -22526,11 +23235,11 @@
       </c>
       <c r="B17" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A17,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>17918</v>
+        <v>9350</v>
       </c>
       <c r="C17" s="20">
         <f>COUNTIFS(Reservas[Estado],A17,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" s="20">
         <f>COUNTIFS(Reservas[Estado],A17,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
@@ -22538,11 +23247,11 @@
       </c>
       <c r="E17" s="24">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="F17" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A17,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>4.5999999999999996</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="16" t="s">
@@ -22553,13 +23262,16 @@
       </c>
       <c r="L17" s="17" t="str">
         <f>IF(M17&gt;0,INDEX(Auxiliar!ListaEstados,MATCH(M17,Auxiliar!ListaVendas,0)),"")</f>
-        <v/>
+        <v>Paraíba</v>
       </c>
       <c r="M17" s="16">
         <f>LARGE(Auxiliar!ListaVendas,K17)</f>
+        <v>5678</v>
+      </c>
+      <c r="N17" s="24">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N17" s="24"/>
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="17" t="s">
@@ -22567,23 +23279,23 @@
       </c>
       <c r="B18" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A18,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>0</v>
+        <v>1450</v>
       </c>
       <c r="C18" s="20">
         <f>COUNTIFS(Reservas[Estado],A18,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="20">
         <f>COUNTIFS(Reservas[Estado],A18,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>0</v>
-      </c>
-      <c r="E18" s="24" t="str">
+        <v>1</v>
+      </c>
+      <c r="E18" s="24">
         <f t="shared" si="0"/>
-        <v>0%</v>
+        <v>1</v>
       </c>
       <c r="F18" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A18,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="16" t="s">
@@ -22594,13 +23306,16 @@
       </c>
       <c r="L18" s="17" t="str">
         <f>IF(M18&gt;0,INDEX(Auxiliar!ListaEstados,MATCH(M18,Auxiliar!ListaVendas,0)),"")</f>
-        <v/>
+        <v>Paraíba</v>
       </c>
       <c r="M18" s="16">
         <f>LARGE(Auxiliar!ListaVendas,K18)</f>
+        <v>5678</v>
+      </c>
+      <c r="N18" s="24">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N18" s="24"/>
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="17" t="s">
@@ -22608,7 +23323,7 @@
       </c>
       <c r="B19" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A19,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>0</v>
+        <v>5678</v>
       </c>
       <c r="C19" s="20">
         <f>COUNTIFS(Reservas[Estado],A19,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
@@ -22616,15 +23331,15 @@
       </c>
       <c r="D19" s="20">
         <f>COUNTIFS(Reservas[Estado],A19,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
+        <v>1</v>
+      </c>
+      <c r="E19" s="24">
+        <f t="shared" si="0"/>
         <v>0</v>
-      </c>
-      <c r="E19" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>0%</v>
       </c>
       <c r="F19" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A19,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H19" s="19"/>
       <c r="I19" s="16" t="s">
@@ -22635,13 +23350,16 @@
       </c>
       <c r="L19" s="17" t="str">
         <f>IF(M19&gt;0,INDEX(Auxiliar!ListaEstados,MATCH(M19,Auxiliar!ListaVendas,0)),"")</f>
-        <v/>
+        <v>Paraná</v>
       </c>
       <c r="M19" s="16">
         <f>LARGE(Auxiliar!ListaVendas,K19)</f>
+        <v>4983</v>
+      </c>
+      <c r="N19" s="24">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N19" s="24"/>
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="17" t="s">
@@ -22649,7 +23367,7 @@
       </c>
       <c r="B20" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A20,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>0</v>
+        <v>4983</v>
       </c>
       <c r="C20" s="20">
         <f>COUNTIFS(Reservas[Estado],A20,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
@@ -22657,15 +23375,15 @@
       </c>
       <c r="D20" s="20">
         <f>COUNTIFS(Reservas[Estado],A20,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
+        <v>1</v>
+      </c>
+      <c r="E20" s="24">
+        <f t="shared" si="0"/>
         <v>0</v>
-      </c>
-      <c r="E20" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>0%</v>
       </c>
       <c r="F20" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A20,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H20" s="19"/>
       <c r="I20" s="16" t="s">
@@ -22678,7 +23396,7 @@
       </c>
       <c r="B21" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A21,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>0</v>
+        <v>21340</v>
       </c>
       <c r="C21" s="20">
         <f>COUNTIFS(Reservas[Estado],A21,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
@@ -22686,15 +23404,15 @@
       </c>
       <c r="D21" s="20">
         <f>COUNTIFS(Reservas[Estado],A21,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
+        <v>4</v>
+      </c>
+      <c r="E21" s="24">
+        <f t="shared" si="0"/>
         <v>0</v>
-      </c>
-      <c r="E21" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>0%</v>
       </c>
       <c r="F21" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A21,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="H21" s="19"/>
       <c r="I21" s="16" t="s">
@@ -22702,7 +23420,7 @@
       </c>
       <c r="K21" s="33" t="str">
         <f>"Análise de Vendas "&amp;Estado</f>
-        <v>Análise de Vendas São Paulo</v>
+        <v>Análise de Vendas Bahia</v>
       </c>
       <c r="L21" s="33"/>
       <c r="M21" s="33"/>
@@ -22714,7 +23432,7 @@
       </c>
       <c r="B22" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A22,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>0</v>
+        <v>1590</v>
       </c>
       <c r="C22" s="20">
         <f>COUNTIFS(Reservas[Estado],A22,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
@@ -22722,15 +23440,15 @@
       </c>
       <c r="D22" s="20">
         <f>COUNTIFS(Reservas[Estado],A22,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
+        <v>1</v>
+      </c>
+      <c r="E22" s="24">
+        <f t="shared" si="0"/>
         <v>0</v>
-      </c>
-      <c r="E22" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>0%</v>
       </c>
       <c r="F22" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A22,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H22" s="19"/>
       <c r="I22" s="16" t="s">
@@ -22755,23 +23473,23 @@
       </c>
       <c r="B23" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A23,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>26160</v>
+        <v>3635</v>
       </c>
       <c r="C23" s="20">
         <f>COUNTIFS(Reservas[Estado],A23,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D23" s="20">
         <f>COUNTIFS(Reservas[Estado],A23,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E23" s="24">
         <f t="shared" si="0"/>
-        <v>0.44444444444444442</v>
+        <v>0.5</v>
       </c>
       <c r="F23" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A23,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>4.666666666666667</v>
+        <v>4.5</v>
       </c>
       <c r="K23" s="26">
         <v>1</v>
@@ -22788,7 +23506,7 @@
       </c>
       <c r="B24" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A24,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>0</v>
+        <v>1660</v>
       </c>
       <c r="C24" s="20">
         <f>COUNTIFS(Reservas[Estado],A24,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
@@ -22796,15 +23514,15 @@
       </c>
       <c r="D24" s="20">
         <f>COUNTIFS(Reservas[Estado],A24,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
+        <v>1</v>
+      </c>
+      <c r="E24" s="24">
+        <f t="shared" si="0"/>
         <v>0</v>
-      </c>
-      <c r="E24" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>0%</v>
       </c>
       <c r="F24" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A24,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H24" s="33" t="s">
         <v>92</v>
@@ -22825,23 +23543,23 @@
       </c>
       <c r="B25" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A25,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>5105</v>
+        <v>5890</v>
       </c>
       <c r="C25" s="20">
         <f>COUNTIFS(Reservas[Estado],A25,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D25" s="20">
         <f>COUNTIFS(Reservas[Estado],A25,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E25" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A25,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H25" s="27" t="s">
         <v>0</v>
@@ -22862,7 +23580,7 @@
       </c>
       <c r="B26" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A26,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>0</v>
+        <v>5678</v>
       </c>
       <c r="C26" s="20">
         <f>COUNTIFS(Reservas[Estado],A26,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
@@ -22870,15 +23588,15 @@
       </c>
       <c r="D26" s="20">
         <f>COUNTIFS(Reservas[Estado],A26,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
+        <v>1</v>
+      </c>
+      <c r="E26" s="24">
+        <f t="shared" si="0"/>
         <v>0</v>
-      </c>
-      <c r="E26" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>0%</v>
       </c>
       <c r="F26" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A26,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H26" s="27" t="s">
         <v>1</v>
@@ -22899,7 +23617,7 @@
       </c>
       <c r="B27" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A27,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>0</v>
+        <v>8765</v>
       </c>
       <c r="C27" s="20">
         <f>COUNTIFS(Reservas[Estado],A27,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
@@ -22907,15 +23625,15 @@
       </c>
       <c r="D27" s="20">
         <f>COUNTIFS(Reservas[Estado],A27,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
+        <v>1</v>
+      </c>
+      <c r="E27" s="24">
+        <f t="shared" si="0"/>
         <v>0</v>
-      </c>
-      <c r="E27" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>0%</v>
       </c>
       <c r="F27" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A27,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H27" s="27" t="s">
         <v>2</v>
@@ -22936,19 +23654,19 @@
       </c>
       <c r="B28" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A28,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>2535</v>
+        <v>11536</v>
       </c>
       <c r="C28" s="20">
         <f>COUNTIFS(Reservas[Estado],A28,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D28" s="20">
         <f>COUNTIFS(Reservas[Estado],A28,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E28" s="24">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F28" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A28,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
@@ -22973,11 +23691,11 @@
       </c>
       <c r="B29" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A29,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>26315</v>
+        <v>20857</v>
       </c>
       <c r="C29" s="20">
         <f>COUNTIFS(Reservas[Estado],A29,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D29" s="20">
         <f>COUNTIFS(Reservas[Estado],A29,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
@@ -22985,11 +23703,11 @@
       </c>
       <c r="E29" s="24">
         <f t="shared" si="0"/>
-        <v>0.44444444444444442</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F29" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A29,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>4.333333333333333</v>
+        <v>4.5555555555555554</v>
       </c>
       <c r="K29" s="26">
         <v>7</v>
@@ -23006,7 +23724,7 @@
       </c>
       <c r="B30" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A30,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>0</v>
+        <v>1730</v>
       </c>
       <c r="C30" s="20">
         <f>COUNTIFS(Reservas[Estado],A30,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
@@ -23014,15 +23732,15 @@
       </c>
       <c r="D30" s="20">
         <f>COUNTIFS(Reservas[Estado],A30,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
+        <v>1</v>
+      </c>
+      <c r="E30" s="24">
+        <f t="shared" si="0"/>
         <v>0</v>
-      </c>
-      <c r="E30" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>0%</v>
       </c>
       <c r="F30" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A30,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H30" s="33" t="s">
         <v>95</v>
@@ -23043,23 +23761,23 @@
       </c>
       <c r="B31" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A31,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>0</v>
+        <v>1800</v>
       </c>
       <c r="C31" s="20">
         <f>COUNTIFS(Reservas[Estado],A31,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31" s="20">
         <f>COUNTIFS(Reservas[Estado],A31,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>0</v>
-      </c>
-      <c r="E31" s="24" t="str">
+        <v>1</v>
+      </c>
+      <c r="E31" s="24">
         <f t="shared" si="0"/>
-        <v>0%</v>
+        <v>1</v>
       </c>
       <c r="F31" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A31,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H31" s="27" t="s">
         <v>0</v>
@@ -23167,7 +23885,7 @@
   </sheetPr>
   <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Q8" sqref="Q7:Q8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Terminando de implementar calculos do dashboard
</commit_message>
<xml_diff>
--- a/dashboards_II.xlsx
+++ b/dashboards_II.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c548d412d6f19400/Área de Trabalho/Alura/excel/Projetos Git/04. DashBoard Especialista/02.Dashboard 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="13_ncr:1_{8621F33A-E581-4B2B-8C24-DD17DCFBD997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C8A0B96-FBE7-4EF5-981A-48572FA5E545}"/>
+  <xr:revisionPtr revIDLastSave="154" documentId="13_ncr:1_{8621F33A-E581-4B2B-8C24-DD17DCFBD997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AFF9C96-C7F0-4FA9-9E94-4CC16526329D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="4" xr2:uid="{18B12833-7551-4467-B611-A6E8F662E40B}"/>
   </bookViews>
@@ -811,6 +811,275 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Auxiliar!$N$10:$N$19</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.38461538461538464</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2731-46F6-B7CB-AFAB3419BD42}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="2086751167"/>
+        <c:axId val="2080678463"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2086751167"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2080678463"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2080678463"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2086751167"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
@@ -871,6 +1140,46 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1418,8 +1727,524 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="16" fmlaLink="Auxiliar!$I$6" fmlaRange="ListaEstados" sel="5" val="3"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="16" fmlaLink="Auxiliar!$I$6" fmlaRange="ListaEstados" sel="19" val="13"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1427,7 +2252,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="12" dropStyle="combo" dx="16" fmlaLink="Auxiliar!$L$5" fmlaRange="ListaMeses" sel="3" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="12" dropStyle="combo" dx="16" fmlaLink="Auxiliar!$L$5" fmlaRange="ListaMeses" sel="10" val="0"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2187,16 +3012,16 @@
   </mc:AlternateContent>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>39220</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>43702</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>344020</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>129427</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>204508</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>509308</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx2="http://schemas.microsoft.com/office/drawing/2015/10/21/chartex" Requires="cx2">
@@ -2205,7 +3030,7 @@
             <xdr:cNvPr id="2" name="Gráfico 1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F307CD2F-5895-68C9-DCA5-0C603B1F512A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2232,7 +3057,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="648820" y="558052"/>
+              <a:off x="344020" y="453277"/>
               <a:ext cx="3213288" cy="1927973"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2261,6 +3086,42 @@
         </xdr:sp>
       </mc:Fallback>
     </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>185458</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>149598</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4D426E5-CC72-9DEE-6236-90D536D5831C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -22654,8 +23515,8 @@
   </sheetPr>
   <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22780,7 +23641,7 @@
       </c>
       <c r="I5" s="35" t="str" cm="1">
         <f t="array" ref="I5">INDEX(Auxiliar!ListaEstados,Auxiliar!IndiceEstado)</f>
-        <v>Bahia</v>
+        <v>Rio de Janeiro</v>
       </c>
       <c r="J5" s="36"/>
       <c r="K5" s="23" cm="1">
@@ -22788,7 +23649,7 @@
         <v>2018</v>
       </c>
       <c r="L5" s="30">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -22819,7 +23680,7 @@
         <v>56</v>
       </c>
       <c r="I6" s="37">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="J6" s="37"/>
       <c r="K6" s="30">
@@ -22950,15 +23811,15 @@
       </c>
       <c r="L10" s="17" t="str">
         <f>IF(M10&gt;0,INDEX(Auxiliar!ListaEstados,MATCH(M10,Auxiliar!ListaVendas,0)),"")</f>
-        <v>Pernambuco</v>
+        <v>São Paulo</v>
       </c>
       <c r="M10" s="16">
         <f>LARGE(Auxiliar!ListaVendas,K10)</f>
-        <v>21340</v>
+        <v>39091</v>
       </c>
       <c r="N10" s="24">
         <f>IFERROR(VLOOKUP(L10,$A$4:$F$31,5,0),"0%")</f>
-        <v>0</v>
+        <v>0.38461538461538464</v>
       </c>
     </row>
     <row r="11" spans="1:19">
@@ -22967,11 +23828,11 @@
       </c>
       <c r="B11" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A11,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>4055</v>
+        <v>11921</v>
       </c>
       <c r="C11" s="20">
         <f>COUNTIFS(Reservas[Estado],A11,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" s="20">
         <f>COUNTIFS(Reservas[Estado],A11,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
@@ -22979,11 +23840,11 @@
       </c>
       <c r="E11" s="24">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F11" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A11,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="H11" s="19">
         <v>2018</v>
@@ -22996,15 +23857,15 @@
       </c>
       <c r="L11" s="17" t="str">
         <f>IF(M11&gt;0,INDEX(Auxiliar!ListaEstados,MATCH(M11,Auxiliar!ListaVendas,0)),"")</f>
-        <v>São Paulo</v>
+        <v>Rio de Janeiro</v>
       </c>
       <c r="M11" s="16">
         <f>LARGE(Auxiliar!ListaVendas,K11)</f>
-        <v>20857</v>
+        <v>32535</v>
       </c>
       <c r="N11" s="24">
         <f t="shared" ref="N11:N19" si="1">IFERROR(VLOOKUP(L11,$A$4:$F$31,5,0),"0%")</f>
-        <v>0.33333333333333331</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -23013,19 +23874,19 @@
       </c>
       <c r="B12" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A12,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>11682</v>
+        <v>16294</v>
       </c>
       <c r="C12" s="20">
         <f>COUNTIFS(Reservas[Estado],A12,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D12" s="20">
         <f>COUNTIFS(Reservas[Estado],A12,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E12" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F12" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A12,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
@@ -23042,15 +23903,15 @@
       </c>
       <c r="L12" s="17" t="str">
         <f>IF(M12&gt;0,INDEX(Auxiliar!ListaEstados,MATCH(M12,Auxiliar!ListaVendas,0)),"")</f>
-        <v>Espírito Santo</v>
+        <v>Minas Gerais</v>
       </c>
       <c r="M12" s="16">
         <f>LARGE(Auxiliar!ListaVendas,K12)</f>
-        <v>11682</v>
+        <v>18677</v>
       </c>
       <c r="N12" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:19">
@@ -23086,11 +23947,11 @@
       </c>
       <c r="L13" s="17" t="str">
         <f>IF(M13&gt;0,INDEX(Auxiliar!ListaEstados,MATCH(M13,Auxiliar!ListaVendas,0)),"")</f>
-        <v>Santa Catarina</v>
+        <v>Rio Grande do Sul</v>
       </c>
       <c r="M13" s="16">
         <f>LARGE(Auxiliar!ListaVendas,K13)</f>
-        <v>11536</v>
+        <v>17732</v>
       </c>
       <c r="N13" s="24">
         <f t="shared" si="1"/>
@@ -23130,15 +23991,15 @@
       </c>
       <c r="L14" s="17" t="str">
         <f>IF(M14&gt;0,INDEX(Auxiliar!ListaEstados,MATCH(M14,Auxiliar!ListaVendas,0)),"")</f>
-        <v>Minas Gerais</v>
+        <v>Espírito Santo</v>
       </c>
       <c r="M14" s="16">
         <f>LARGE(Auxiliar!ListaVendas,K14)</f>
-        <v>9350</v>
+        <v>16294</v>
       </c>
       <c r="N14" s="24">
         <f t="shared" si="1"/>
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:19">
@@ -23147,23 +24008,23 @@
       </c>
       <c r="B15" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A15,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>1345</v>
+        <v>0</v>
       </c>
       <c r="C15" s="20">
         <f>COUNTIFS(Reservas[Estado],A15,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" s="20">
         <f>COUNTIFS(Reservas[Estado],A15,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>1</v>
-      </c>
-      <c r="E15" s="24">
+        <v>0</v>
+      </c>
+      <c r="E15" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0%</v>
       </c>
       <c r="F15" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A15,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="16" t="s">
@@ -23174,11 +24035,11 @@
       </c>
       <c r="L15" s="17" t="str">
         <f>IF(M15&gt;0,INDEX(Auxiliar!ListaEstados,MATCH(M15,Auxiliar!ListaVendas,0)),"")</f>
-        <v>Roraima</v>
+        <v>Distrito Federal</v>
       </c>
       <c r="M15" s="16">
         <f>LARGE(Auxiliar!ListaVendas,K15)</f>
-        <v>8765</v>
+        <v>11921</v>
       </c>
       <c r="N15" s="24">
         <f t="shared" si="1"/>
@@ -23191,7 +24052,7 @@
       </c>
       <c r="B16" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A16,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>1380</v>
+        <v>0</v>
       </c>
       <c r="C16" s="20">
         <f>COUNTIFS(Reservas[Estado],A16,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
@@ -23199,15 +24060,15 @@
       </c>
       <c r="D16" s="20">
         <f>COUNTIFS(Reservas[Estado],A16,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>1</v>
-      </c>
-      <c r="E16" s="24">
+        <v>0</v>
+      </c>
+      <c r="E16" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0%</v>
       </c>
       <c r="F16" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A16,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="16" t="s">
@@ -23218,15 +24079,15 @@
       </c>
       <c r="L16" s="17" t="str">
         <f>IF(M16&gt;0,INDEX(Auxiliar!ListaEstados,MATCH(M16,Auxiliar!ListaVendas,0)),"")</f>
-        <v>Rio Grande do Sul</v>
+        <v>Santa Catarina</v>
       </c>
       <c r="M16" s="16">
         <f>LARGE(Auxiliar!ListaVendas,K16)</f>
-        <v>5890</v>
+        <v>7896</v>
       </c>
       <c r="N16" s="24">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:14">
@@ -23235,23 +24096,23 @@
       </c>
       <c r="B17" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A17,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>9350</v>
+        <v>18677</v>
       </c>
       <c r="C17" s="20">
         <f>COUNTIFS(Reservas[Estado],A17,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D17" s="20">
         <f>COUNTIFS(Reservas[Estado],A17,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E17" s="24">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="F17" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A17,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>4.4000000000000004</v>
+        <v>4.833333333333333</v>
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="16" t="s">
@@ -23262,11 +24123,11 @@
       </c>
       <c r="L17" s="17" t="str">
         <f>IF(M17&gt;0,INDEX(Auxiliar!ListaEstados,MATCH(M17,Auxiliar!ListaVendas,0)),"")</f>
-        <v>Paraíba</v>
+        <v>Pernambuco</v>
       </c>
       <c r="M17" s="16">
         <f>LARGE(Auxiliar!ListaVendas,K17)</f>
-        <v>5678</v>
+        <v>2430</v>
       </c>
       <c r="N17" s="24">
         <f t="shared" si="1"/>
@@ -23279,23 +24140,23 @@
       </c>
       <c r="B18" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A18,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>1450</v>
+        <v>0</v>
       </c>
       <c r="C18" s="20">
         <f>COUNTIFS(Reservas[Estado],A18,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" s="20">
         <f>COUNTIFS(Reservas[Estado],A18,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>1</v>
-      </c>
-      <c r="E18" s="24">
+        <v>0</v>
+      </c>
+      <c r="E18" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0%</v>
       </c>
       <c r="F18" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A18,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="16" t="s">
@@ -23306,15 +24167,15 @@
       </c>
       <c r="L18" s="17" t="str">
         <f>IF(M18&gt;0,INDEX(Auxiliar!ListaEstados,MATCH(M18,Auxiliar!ListaVendas,0)),"")</f>
-        <v>Paraíba</v>
+        <v/>
       </c>
       <c r="M18" s="16">
         <f>LARGE(Auxiliar!ListaVendas,K18)</f>
-        <v>5678</v>
-      </c>
-      <c r="N18" s="24">
+        <v>0</v>
+      </c>
+      <c r="N18" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0%</v>
       </c>
     </row>
     <row r="19" spans="1:14">
@@ -23323,7 +24184,7 @@
       </c>
       <c r="B19" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A19,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>5678</v>
+        <v>0</v>
       </c>
       <c r="C19" s="20">
         <f>COUNTIFS(Reservas[Estado],A19,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
@@ -23331,15 +24192,15 @@
       </c>
       <c r="D19" s="20">
         <f>COUNTIFS(Reservas[Estado],A19,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>1</v>
-      </c>
-      <c r="E19" s="24">
+        <v>0</v>
+      </c>
+      <c r="E19" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0%</v>
       </c>
       <c r="F19" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A19,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H19" s="19"/>
       <c r="I19" s="16" t="s">
@@ -23350,15 +24211,15 @@
       </c>
       <c r="L19" s="17" t="str">
         <f>IF(M19&gt;0,INDEX(Auxiliar!ListaEstados,MATCH(M19,Auxiliar!ListaVendas,0)),"")</f>
-        <v>Paraná</v>
+        <v/>
       </c>
       <c r="M19" s="16">
         <f>LARGE(Auxiliar!ListaVendas,K19)</f>
-        <v>4983</v>
-      </c>
-      <c r="N19" s="24">
+        <v>0</v>
+      </c>
+      <c r="N19" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0%</v>
       </c>
     </row>
     <row r="20" spans="1:14">
@@ -23367,7 +24228,7 @@
       </c>
       <c r="B20" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A20,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>4983</v>
+        <v>0</v>
       </c>
       <c r="C20" s="20">
         <f>COUNTIFS(Reservas[Estado],A20,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
@@ -23375,15 +24236,15 @@
       </c>
       <c r="D20" s="20">
         <f>COUNTIFS(Reservas[Estado],A20,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>1</v>
-      </c>
-      <c r="E20" s="24">
+        <v>0</v>
+      </c>
+      <c r="E20" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0%</v>
       </c>
       <c r="F20" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A20,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H20" s="19"/>
       <c r="I20" s="16" t="s">
@@ -23396,7 +24257,7 @@
       </c>
       <c r="B21" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A21,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>21340</v>
+        <v>2430</v>
       </c>
       <c r="C21" s="20">
         <f>COUNTIFS(Reservas[Estado],A21,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
@@ -23404,7 +24265,7 @@
       </c>
       <c r="D21" s="20">
         <f>COUNTIFS(Reservas[Estado],A21,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E21" s="24">
         <f t="shared" si="0"/>
@@ -23412,7 +24273,7 @@
       </c>
       <c r="F21" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A21,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="H21" s="19"/>
       <c r="I21" s="16" t="s">
@@ -23420,7 +24281,7 @@
       </c>
       <c r="K21" s="33" t="str">
         <f>"Análise de Vendas "&amp;Estado</f>
-        <v>Análise de Vendas Bahia</v>
+        <v>Análise de Vendas Rio de Janeiro</v>
       </c>
       <c r="L21" s="33"/>
       <c r="M21" s="33"/>
@@ -23432,7 +24293,7 @@
       </c>
       <c r="B22" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A22,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>1590</v>
+        <v>0</v>
       </c>
       <c r="C22" s="20">
         <f>COUNTIFS(Reservas[Estado],A22,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
@@ -23440,15 +24301,15 @@
       </c>
       <c r="D22" s="20">
         <f>COUNTIFS(Reservas[Estado],A22,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>1</v>
-      </c>
-      <c r="E22" s="24">
+        <v>0</v>
+      </c>
+      <c r="E22" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0%</v>
       </c>
       <c r="F22" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A22,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H22" s="19"/>
       <c r="I22" s="16" t="s">
@@ -23473,23 +24334,23 @@
       </c>
       <c r="B23" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A23,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>3635</v>
+        <v>32535</v>
       </c>
       <c r="C23" s="20">
         <f>COUNTIFS(Reservas[Estado],A23,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23" s="20">
         <f>COUNTIFS(Reservas[Estado],A23,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E23" s="24">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="F23" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A23,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>4.5</v>
+        <v>4.3</v>
       </c>
       <c r="K23" s="26">
         <v>1</v>
@@ -23497,8 +24358,14 @@
       <c r="L23" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="M23" s="16"/>
-      <c r="N23" s="20"/>
+      <c r="M23" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],Auxiliar!Estado,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],K23)</f>
+        <v>3915</v>
+      </c>
+      <c r="N23" s="20">
+        <f>COUNTIFS(Reservas[Estado],Auxiliar!Estado,Reservas[Ano],Ano,Reservas[Mês],K23)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="24" spans="1:14">
       <c r="A24" s="17" t="s">
@@ -23506,7 +24373,7 @@
       </c>
       <c r="B24" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A24,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>1660</v>
+        <v>0</v>
       </c>
       <c r="C24" s="20">
         <f>COUNTIFS(Reservas[Estado],A24,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
@@ -23514,15 +24381,15 @@
       </c>
       <c r="D24" s="20">
         <f>COUNTIFS(Reservas[Estado],A24,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>1</v>
-      </c>
-      <c r="E24" s="24">
+        <v>0</v>
+      </c>
+      <c r="E24" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0%</v>
       </c>
       <c r="F24" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A24,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H24" s="33" t="s">
         <v>92</v>
@@ -23534,8 +24401,14 @@
       <c r="L24" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="M24" s="16"/>
-      <c r="N24" s="20"/>
+      <c r="M24" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],Auxiliar!Estado,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],K24)</f>
+        <v>33513</v>
+      </c>
+      <c r="N24" s="20">
+        <f>COUNTIFS(Reservas[Estado],Auxiliar!Estado,Reservas[Ano],Ano,Reservas[Mês],K24)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="25" spans="1:14">
       <c r="A25" s="17" t="s">
@@ -23543,36 +24416,45 @@
       </c>
       <c r="B25" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A25,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>5890</v>
+        <v>17732</v>
       </c>
       <c r="C25" s="20">
         <f>COUNTIFS(Reservas[Estado],A25,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D25" s="20">
         <f>COUNTIFS(Reservas[Estado],A25,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E25" s="24">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A25,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="H25" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="I25" s="16"/>
+      <c r="I25" s="16">
+        <f>SUMIFS(Reservas[Valor Total], Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Vendedor],H25)</f>
+        <v>38668</v>
+      </c>
       <c r="K25" s="26">
         <v>3</v>
       </c>
       <c r="L25" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="M25" s="16"/>
-      <c r="N25" s="20"/>
+      <c r="M25" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],Auxiliar!Estado,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],K25)</f>
+        <v>3635</v>
+      </c>
+      <c r="N25" s="20">
+        <f>COUNTIFS(Reservas[Estado],Auxiliar!Estado,Reservas[Ano],Ano,Reservas[Mês],K25)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="26" spans="1:14">
       <c r="A26" s="17" t="s">
@@ -23580,7 +24462,7 @@
       </c>
       <c r="B26" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A26,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>5678</v>
+        <v>0</v>
       </c>
       <c r="C26" s="20">
         <f>COUNTIFS(Reservas[Estado],A26,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
@@ -23588,28 +24470,37 @@
       </c>
       <c r="D26" s="20">
         <f>COUNTIFS(Reservas[Estado],A26,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>1</v>
-      </c>
-      <c r="E26" s="24">
+        <v>0</v>
+      </c>
+      <c r="E26" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0%</v>
       </c>
       <c r="F26" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A26,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H26" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="I26" s="16"/>
+      <c r="I26" s="16">
+        <f>SUMIFS(Reservas[Valor Total], Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Vendedor],H26)</f>
+        <v>38673</v>
+      </c>
       <c r="K26" s="26">
         <v>4</v>
       </c>
       <c r="L26" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="M26" s="16"/>
-      <c r="N26" s="20"/>
+      <c r="M26" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],Auxiliar!Estado,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],K26)</f>
+        <v>48244</v>
+      </c>
+      <c r="N26" s="20">
+        <f>COUNTIFS(Reservas[Estado],Auxiliar!Estado,Reservas[Ano],Ano,Reservas[Mês],K26)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="17" t="s">
@@ -23617,7 +24508,7 @@
       </c>
       <c r="B27" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A27,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>8765</v>
+        <v>0</v>
       </c>
       <c r="C27" s="20">
         <f>COUNTIFS(Reservas[Estado],A27,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
@@ -23625,28 +24516,37 @@
       </c>
       <c r="D27" s="20">
         <f>COUNTIFS(Reservas[Estado],A27,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>1</v>
-      </c>
-      <c r="E27" s="24">
+        <v>0</v>
+      </c>
+      <c r="E27" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0%</v>
       </c>
       <c r="F27" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A27,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H27" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="I27" s="16"/>
+      <c r="I27" s="16">
+        <f>SUMIFS(Reservas[Valor Total], Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Vendedor],H27)</f>
+        <v>33094</v>
+      </c>
       <c r="K27" s="26">
         <v>5</v>
       </c>
       <c r="L27" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="M27" s="16"/>
-      <c r="N27" s="20"/>
+      <c r="M27" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],Auxiliar!Estado,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],K27)</f>
+        <v>4510</v>
+      </c>
+      <c r="N27" s="20">
+        <f>COUNTIFS(Reservas[Estado],Auxiliar!Estado,Reservas[Ano],Ano,Reservas[Mês],K27)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="28" spans="1:14">
       <c r="A28" s="17" t="s">
@@ -23654,7 +24554,7 @@
       </c>
       <c r="B28" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A28,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>11536</v>
+        <v>7896</v>
       </c>
       <c r="C28" s="20">
         <f>COUNTIFS(Reservas[Estado],A28,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
@@ -23662,7 +24562,7 @@
       </c>
       <c r="D28" s="20">
         <f>COUNTIFS(Reservas[Estado],A28,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E28" s="24">
         <f t="shared" si="0"/>
@@ -23675,15 +24575,24 @@
       <c r="H28" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="I28" s="16"/>
+      <c r="I28" s="16">
+        <f>SUMIFS(Reservas[Valor Total], Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Vendedor],H28)</f>
+        <v>36141</v>
+      </c>
       <c r="K28" s="26">
         <v>6</v>
       </c>
       <c r="L28" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="M28" s="16"/>
-      <c r="N28" s="20"/>
+      <c r="M28" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],Auxiliar!Estado,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],K28)</f>
+        <v>33470</v>
+      </c>
+      <c r="N28" s="20">
+        <f>COUNTIFS(Reservas[Estado],Auxiliar!Estado,Reservas[Ano],Ano,Reservas[Mês],K28)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="29" spans="1:14">
       <c r="A29" s="17" t="s">
@@ -23691,23 +24600,23 @@
       </c>
       <c r="B29" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A29,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>20857</v>
+        <v>39091</v>
       </c>
       <c r="C29" s="20">
         <f>COUNTIFS(Reservas[Estado],A29,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D29" s="20">
         <f>COUNTIFS(Reservas[Estado],A29,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E29" s="24">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.38461538461538464</v>
       </c>
       <c r="F29" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A29,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>4.5555555555555554</v>
+        <v>4.615384615384615</v>
       </c>
       <c r="K29" s="26">
         <v>7</v>
@@ -23715,8 +24624,14 @@
       <c r="L29" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="M29" s="16"/>
-      <c r="N29" s="20"/>
+      <c r="M29" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],Auxiliar!Estado,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],K29)</f>
+        <v>2345</v>
+      </c>
+      <c r="N29" s="20">
+        <f>COUNTIFS(Reservas[Estado],Auxiliar!Estado,Reservas[Ano],Ano,Reservas[Mês],K29)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:14">
       <c r="A30" s="17" t="s">
@@ -23724,7 +24639,7 @@
       </c>
       <c r="B30" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A30,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>1730</v>
+        <v>0</v>
       </c>
       <c r="C30" s="20">
         <f>COUNTIFS(Reservas[Estado],A30,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
@@ -23732,15 +24647,15 @@
       </c>
       <c r="D30" s="20">
         <f>COUNTIFS(Reservas[Estado],A30,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>1</v>
-      </c>
-      <c r="E30" s="24">
+        <v>0</v>
+      </c>
+      <c r="E30" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0%</v>
       </c>
       <c r="F30" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A30,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H30" s="33" t="s">
         <v>95</v>
@@ -23752,8 +24667,14 @@
       <c r="L30" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="M30" s="16"/>
-      <c r="N30" s="20"/>
+      <c r="M30" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],Auxiliar!Estado,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],K30)</f>
+        <v>26160</v>
+      </c>
+      <c r="N30" s="20">
+        <f>COUNTIFS(Reservas[Estado],Auxiliar!Estado,Reservas[Ano],Ano,Reservas[Mês],K30)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="31" spans="1:14">
       <c r="A31" s="17" t="s">
@@ -23761,78 +24682,114 @@
       </c>
       <c r="B31" s="16">
         <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],A31,Reservas[Ano],Ano,Reservas[Mês],Mes)</f>
-        <v>1800</v>
+        <v>0</v>
       </c>
       <c r="C31" s="20">
         <f>COUNTIFS(Reservas[Estado],A31,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Status],"Cancelada")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D31" s="20">
         <f>COUNTIFS(Reservas[Estado],A31,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes)</f>
-        <v>1</v>
-      </c>
-      <c r="E31" s="24">
+        <v>0</v>
+      </c>
+      <c r="E31" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0%</v>
       </c>
       <c r="F31" s="25">
         <f>IFERROR(AVERAGEIFS(Reservas[Avaliação],Reservas[Estado],A31,Reservas[Ano],Ano,Reservas[Mês],Auxiliar!Mes),0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H31" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="I31" s="16"/>
+      <c r="I31" s="16">
+        <f>SUMIFS(Reservas[Comissão], Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Vendedor],H31)</f>
+        <v>1933.3999999999999</v>
+      </c>
       <c r="K31" s="26">
         <v>9</v>
       </c>
       <c r="L31" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="M31" s="16"/>
-      <c r="N31" s="20"/>
+      <c r="M31" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],Auxiliar!Estado,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],K31)</f>
+        <v>16373</v>
+      </c>
+      <c r="N31" s="20">
+        <f>COUNTIFS(Reservas[Estado],Auxiliar!Estado,Reservas[Ano],Ano,Reservas[Mês],K31)</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="32" spans="1:14">
       <c r="H32" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="I32" s="16"/>
+      <c r="I32" s="16">
+        <f>SUMIFS(Reservas[Comissão], Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Vendedor],H32)</f>
+        <v>1933.65</v>
+      </c>
       <c r="K32" s="26">
         <v>10</v>
       </c>
       <c r="L32" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="M32" s="16"/>
-      <c r="N32" s="20"/>
+      <c r="M32" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],Auxiliar!Estado,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],K32)</f>
+        <v>32535</v>
+      </c>
+      <c r="N32" s="20">
+        <f>COUNTIFS(Reservas[Estado],Auxiliar!Estado,Reservas[Ano],Ano,Reservas[Mês],K32)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="33" spans="8:14">
       <c r="H33" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="I33" s="16"/>
+      <c r="I33" s="16">
+        <f>SUMIFS(Reservas[Comissão], Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Vendedor],H33)</f>
+        <v>1654.7</v>
+      </c>
       <c r="K33" s="26">
         <v>11</v>
       </c>
       <c r="L33" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="M33" s="16"/>
-      <c r="N33" s="20"/>
+      <c r="M33" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],Auxiliar!Estado,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],K33)</f>
+        <v>6100</v>
+      </c>
+      <c r="N33" s="20">
+        <f>COUNTIFS(Reservas[Estado],Auxiliar!Estado,Reservas[Ano],Ano,Reservas[Mês],K33)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="34" spans="8:14">
       <c r="H34" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="I34" s="16"/>
+      <c r="I34" s="16">
+        <f>SUMIFS(Reservas[Comissão], Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Vendedor],H34)</f>
+        <v>1807.05</v>
+      </c>
       <c r="K34" s="26">
         <v>12</v>
       </c>
       <c r="L34" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="M34" s="16"/>
-      <c r="N34" s="20"/>
+      <c r="M34" s="16">
+        <f>SUMIFS(Reservas[Valor Total],Reservas[Estado],Auxiliar!Estado,Reservas[Ano],Auxiliar!Ano,Reservas[Mês],K34)</f>
+        <v>21510</v>
+      </c>
+      <c r="N34" s="20">
+        <f>COUNTIFS(Reservas[Estado],Auxiliar!Estado,Reservas[Ano],Ano,Reservas[Mês],K34)</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="36" spans="8:14">
       <c r="H36" s="33" t="s">
@@ -23844,19 +24801,28 @@
       <c r="H37" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="I37" s="16"/>
+      <c r="I37" s="16">
+        <f>SUMIFS(Reservas[Valor Total], Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Forma Pagamento],H37)</f>
+        <v>106988</v>
+      </c>
     </row>
     <row r="38" spans="8:14">
       <c r="H38" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="I38" s="16"/>
+      <c r="I38" s="16">
+        <f>SUMIFS(Reservas[Valor Total], Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Forma Pagamento],H38)</f>
+        <v>21993</v>
+      </c>
     </row>
     <row r="39" spans="8:14">
       <c r="H39" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="I39" s="16"/>
+      <c r="I39" s="16">
+        <f>SUMIFS(Reservas[Valor Total], Reservas[Ano],Auxiliar!Ano,Reservas[Mês],Auxiliar!Mes,Reservas[Forma Pagamento],H39)</f>
+        <v>17595</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -23886,7 +24852,7 @@
   <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q7:Q8"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Finalizando graficos do dashboard
</commit_message>
<xml_diff>
--- a/dashboards_II.xlsx
+++ b/dashboards_II.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c548d412d6f19400/Área de Trabalho/Alura/excel/Projetos Git/04. DashBoard Especialista/02.Dashboard 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="154" documentId="13_ncr:1_{8621F33A-E581-4B2B-8C24-DD17DCFBD997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AFF9C96-C7F0-4FA9-9E94-4CC16526329D}"/>
+  <xr:revisionPtr revIDLastSave="173" documentId="13_ncr:1_{8621F33A-E581-4B2B-8C24-DD17DCFBD997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD57A73E-1FCE-4B47-B381-73D088E70BC3}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="4" xr2:uid="{18B12833-7551-4467-B611-A6E8F662E40B}"/>
   </bookViews>
@@ -1080,6 +1080,1371 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-4DB8-4BF3-BD0A-EBBAD30CC9AF}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-4DB8-4BF3-BD0A-EBBAD30CC9AF}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-4DB8-4BF3-BD0A-EBBAD30CC9AF}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Auxiliar!$H$37:$H$39</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Cartão de Crédito</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Boleto Bancário</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Depósito Bancário</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Auxiliar!$I$37:$I$39</c:f>
+              <c:numCache>
+                <c:formatCode>_-"R$"\ * #,##0_-;\-"R$"\ * #,##0_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>106988</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21993</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17595</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-4DB8-4BF3-BD0A-EBBAD30CC9AF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-AA12-4709-B446-127D991F0310}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-AA12-4709-B446-127D991F0310}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-AA12-4709-B446-127D991F0310}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-AA12-4709-B446-127D991F0310}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="bestFit"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Auxiliar!$H$25:$H$28</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Priscila</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Carlos</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Letícia</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Patrícia</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Auxiliar!$I$25:$I$28</c:f>
+              <c:numCache>
+                <c:formatCode>_-"R$"\ * #,##0_-;\-"R$"\ * #,##0_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>38668</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38673</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33094</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36141</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-AA12-4709-B446-127D991F0310}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="bestFit"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-BE75-4641-9E94-C65894C14EA8}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-BE75-4641-9E94-C65894C14EA8}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-BE75-4641-9E94-C65894C14EA8}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-BE75-4641-9E94-C65894C14EA8}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="bestFit"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Auxiliar!$H$31:$H$34</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Priscila</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Carlos</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Letícia</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Patrícia</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Auxiliar!$I$31:$I$34</c:f>
+              <c:numCache>
+                <c:formatCode>_-"R$"\ * #,##0_-;\-"R$"\ * #,##0_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1933.3999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1933.65</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1654.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1807.05</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-BE75-4641-9E94-C65894C14EA8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="bestFit"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Auxiliar!$L$23:$L$34</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Fev</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Abr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Mai</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Ago</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Set</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Out</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Dez</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Auxiliar!$M$23:$M$34</c:f>
+              <c:numCache>
+                <c:formatCode>_-"R$"\ * #,##0_-;\-"R$"\ * #,##0_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>3915</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33513</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3635</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>48244</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4510</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>33470</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2345</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26160</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16373</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32535</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>21510</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1F8D-4806-AFA9-55DD6FB3A819}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2061097151"/>
+        <c:axId val="954871951"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Auxiliar!$L$23:$L$34</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Fev</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Abr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Mai</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Ago</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Set</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Out</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Dez</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Auxiliar!$N$23:$N$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1F8D-4806-AFA9-55DD6FB3A819}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2061094751"/>
+        <c:axId val="954874431"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2061097151"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="954871951"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="954871951"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2061097151"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="954874431"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2061094751"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="2061094751"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="954874431"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
@@ -1180,6 +2545,166 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2243,6 +3768,2079 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="322">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="16" fmlaLink="Auxiliar!$I$6" fmlaRange="ListaEstados" sel="19" val="13"/>
 </file>
@@ -3106,7 +6704,7 @@
         <xdr:cNvPr id="3" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4D426E5-CC72-9DEE-6236-90D536D5831C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3119,6 +6717,150 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>248210</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>14007</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E27A9F19-E3C8-ED6B-3DE2-3D8C90F6158B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>200586</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>66676</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>109256</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC9A639B-08DF-17C8-1F0D-4EC4F7F3635F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>219635</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D300D3E1-6A24-7C52-2BC0-63F4F66CA999}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>248209</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>127186</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>504824</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Gráfico 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36C724BE-F6A6-D510-C343-AD24DCB63E47}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -23516,7 +27258,7 @@
   <dimension ref="A1:S39"/>
   <sheetViews>
     <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+      <selection activeCell="L23" sqref="L23:N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -24852,7 +28594,7 @@
   <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>